<commit_message>
updated parameters in config files
</commit_message>
<xml_diff>
--- a/gcam/input/biochar_land_R/GCAM_parameters.xlsx
+++ b/gcam/input/biochar_land_R/GCAM_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natha\PycharmProjects\IAM\biochar\gcam\input\biochar_land_R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{680C30CC-8CE9-4943-B366-650EEB3796ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8A341BD-C680-4A01-801F-9DACECAAC689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{D3FBB104-BEF4-4FDA-A1FA-9751FB33CA85}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="17385" xr2:uid="{D3FBB104-BEF4-4FDA-A1FA-9751FB33CA85}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="123">
   <si>
     <t>Name</t>
   </si>
@@ -131,21 +131,6 @@
     <t>Poultry Biochar Cost</t>
   </si>
   <si>
-    <t>Beef Biochar Sequestered C</t>
-  </si>
-  <si>
-    <t>Dairy Biochar Sequestered C</t>
-  </si>
-  <si>
-    <t>Goat Biochar Sequestered C</t>
-  </si>
-  <si>
-    <t>Pork Biochar Sequestered C</t>
-  </si>
-  <si>
-    <t>Poultry Biochar Sequestered C</t>
-  </si>
-  <si>
     <t>CH4 reduced emissions in land managed with biochar</t>
   </si>
   <si>
@@ -263,30 +248,12 @@
     <t>Poultry Biochar Avoided N2O</t>
   </si>
   <si>
-    <t>kg CO2/kg biochar</t>
-  </si>
-  <si>
     <t>kg CH4/kg biochar</t>
   </si>
   <si>
     <t>kg N2O/kg biochar</t>
   </si>
   <si>
-    <t>Beef Biochar Net CO2 Emissions</t>
-  </si>
-  <si>
-    <t>Dairy Biochar Net CO2 Emissions</t>
-  </si>
-  <si>
-    <t>Goat Biochar Net CO2 Emissions</t>
-  </si>
-  <si>
-    <t>Pork Biochar Net CO2 Emissions</t>
-  </si>
-  <si>
-    <t>Poultry Biochar Net CO2 Emissions</t>
-  </si>
-  <si>
     <t>Results from TEA excel sheet</t>
   </si>
   <si>
@@ -423,6 +390,21 @@
   </si>
   <si>
     <t>A_agBiocharCropYieldIncrease</t>
+  </si>
+  <si>
+    <t>Beef Biochar Net C</t>
+  </si>
+  <si>
+    <t>Dairy Biochar Net C</t>
+  </si>
+  <si>
+    <t>Goat Biochar Net C</t>
+  </si>
+  <si>
+    <t>Pork Biochar Net C</t>
+  </si>
+  <si>
+    <t>Poultry Biochar Net C</t>
   </si>
 </sst>
 </file>
@@ -430,9 +412,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="173" formatCode="0.000"/>
-    <numFmt numFmtId="174" formatCode="0.00000"/>
-    <numFmt numFmtId="175" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.00000"/>
+    <numFmt numFmtId="166" formatCode="0.0%"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -582,16 +564,16 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="173" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="174" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="175" fontId="2" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -929,10 +911,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FC7B4C1-BB5E-45EB-9034-E2CB0DD15D7E}">
-  <dimension ref="A1:H70"/>
+  <dimension ref="A1:H65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -961,16 +943,16 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -989,16 +971,16 @@
         <v>3.8834999999999997</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1017,16 +999,16 @@
         <v>2.6999999999999996E-2</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1045,16 +1027,16 @@
         <v>4.6515000000000004</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1073,16 +1055,16 @@
         <v>0.45599999999999996</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1101,16 +1083,16 @@
         <v>2.0714999999999999</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1128,16 +1110,16 @@
         <v>0.502</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
@@ -1156,16 +1138,16 @@
         <v>1.2209999999999999E-2</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="F8" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="H8" s="11" t="s">
         <v>91</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="H8" s="11" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
@@ -1184,16 +1166,16 @@
         <v>8.0999999999999996E-4</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="F9" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="H9" s="11" t="s">
         <v>91</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="H9" s="11" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1211,17 +1193,17 @@
         <v>0.502</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="G10" s="7" t="str">
         <f>G7</f>
         <v>low value is the lowest value reported in the paper, default is the highest value. Difference between the 2 reported values is added to the default value to calculate the high value</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
@@ -1241,16 +1223,16 @@
         <v>1.2209999999999999E-2</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="F11" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="H11" s="11" t="s">
         <v>91</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="H11" s="11" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
@@ -1270,16 +1252,16 @@
         <v>8.0999999999999996E-4</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="F12" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="H12" s="11" t="s">
         <v>91</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="H12" s="11" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
@@ -1296,16 +1278,16 @@
         <v>0.56110000000000004</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="G13" s="7" t="s">
         <v>11</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1324,16 +1306,16 @@
         <v>5.2500000000000003E-3</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="H14" s="11" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1352,16 +1334,16 @@
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="H15" s="11" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
@@ -1378,16 +1360,16 @@
         <v>0.54679999999999995</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="G16" s="7" t="s">
         <v>11</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
@@ -1404,16 +1386,16 @@
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="G17" s="7" t="s">
         <v>11</v>
       </c>
       <c r="H17" s="11" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
@@ -1430,16 +1412,16 @@
         <v>3.1E-2</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="G18" s="7" t="s">
         <v>11</v>
       </c>
       <c r="H18" s="11" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1456,16 +1438,16 @@
         <v>0.53259999999999996</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="G19" s="7" t="s">
         <v>11</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
@@ -1484,16 +1466,16 @@
         <v>2.8299999999999999E-2</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="H20" s="11" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
@@ -1512,16 +1494,16 @@
         <v>7.46E-2</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="H21" s="11" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1529,25 +1511,25 @@
         <v>26</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1555,25 +1537,25 @@
         <v>27</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1581,25 +1563,25 @@
         <v>28</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1607,25 +1589,25 @@
         <v>29</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1633,30 +1615,30 @@
         <v>30</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
-        <v>31</v>
+        <v>118</v>
       </c>
       <c r="B27" s="12">
         <f>0.5*C27</f>
@@ -1670,49 +1652,49 @@
         <v>-0.375</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
-        <v>32</v>
+        <v>119</v>
       </c>
       <c r="B28" s="12">
-        <f t="shared" ref="B28:B48" si="2">0.5*C28</f>
+        <f t="shared" ref="B28:B43" si="2">0.5*C28</f>
         <v>-0.125</v>
       </c>
       <c r="C28" s="12">
         <v>-0.25</v>
       </c>
       <c r="D28" s="12">
-        <f t="shared" ref="D28:D48" si="3">1.5*C28</f>
+        <f t="shared" ref="D28:D43" si="3">1.5*C28</f>
         <v>-0.375</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
-        <v>33</v>
+        <v>120</v>
       </c>
       <c r="B29" s="12">
         <f t="shared" si="2"/>
@@ -1726,21 +1708,21 @@
         <v>-0.46499999999999997</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="6" t="s">
-        <v>34</v>
+        <v>121</v>
       </c>
       <c r="B30" s="12">
         <f t="shared" si="2"/>
@@ -1754,21 +1736,21 @@
         <v>-0.46499999999999997</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
-        <v>35</v>
+        <v>122</v>
       </c>
       <c r="B31" s="12">
         <f t="shared" si="2"/>
@@ -1782,156 +1764,156 @@
         <v>-0.42000000000000004</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="B32" s="13">
         <f t="shared" si="2"/>
-        <v>-0.38750000000000001</v>
+        <v>-5.3E-3</v>
       </c>
       <c r="C32" s="13">
-        <v>-0.77500000000000002</v>
+        <v>-1.06E-2</v>
       </c>
       <c r="D32" s="13">
         <f t="shared" si="3"/>
-        <v>-1.1625000000000001</v>
+        <v>-1.5900000000000001E-2</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F32" s="11" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="B33" s="13">
         <f t="shared" si="2"/>
-        <v>-0.38750000000000001</v>
+        <v>-5.3E-3</v>
       </c>
       <c r="C33" s="13">
-        <v>-0.77500000000000002</v>
+        <v>-1.06E-2</v>
       </c>
       <c r="D33" s="13">
         <f t="shared" si="3"/>
-        <v>-1.1625000000000001</v>
+        <v>-1.5900000000000001E-2</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="B34" s="13">
         <f t="shared" si="2"/>
-        <v>-0.39650000000000002</v>
+        <v>-5.1150000000000001E-2</v>
       </c>
       <c r="C34" s="13">
-        <v>-0.79300000000000004</v>
+        <v>-0.1023</v>
       </c>
       <c r="D34" s="13">
         <f t="shared" si="3"/>
-        <v>-1.1895</v>
+        <v>-0.15345</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F34" s="11" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="B35" s="13">
         <f t="shared" si="2"/>
-        <v>-0.39650000000000002</v>
+        <v>-5.1150000000000001E-2</v>
       </c>
       <c r="C35" s="13">
-        <v>-0.79300000000000004</v>
+        <v>-0.1023</v>
       </c>
       <c r="D35" s="13">
         <f t="shared" si="3"/>
-        <v>-1.1895</v>
+        <v>-0.15345</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F35" s="11" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="B36" s="13">
-        <f>0.5*C36</f>
-        <v>-0.45100000000000001</v>
+        <f t="shared" si="2"/>
+        <v>-2.8500000000000001E-3</v>
       </c>
       <c r="C36" s="13">
-        <v>-0.90200000000000002</v>
+        <v>-5.7000000000000002E-3</v>
       </c>
       <c r="D36" s="13">
         <f t="shared" si="3"/>
-        <v>-1.353</v>
+        <v>-8.5500000000000003E-3</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F36" s="11" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
@@ -1940,26 +1922,26 @@
       </c>
       <c r="B37" s="13">
         <f t="shared" si="2"/>
-        <v>-5.3E-3</v>
+        <v>-2.5999999999999998E-4</v>
       </c>
       <c r="C37" s="13">
-        <v>-1.06E-2</v>
+        <v>-5.1999999999999995E-4</v>
       </c>
       <c r="D37" s="13">
         <f t="shared" si="3"/>
-        <v>-1.5900000000000001E-2</v>
+        <v>-7.7999999999999988E-4</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="F37" s="11" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
@@ -1968,26 +1950,26 @@
       </c>
       <c r="B38" s="13">
         <f t="shared" si="2"/>
-        <v>-5.3E-3</v>
+        <v>-2.5999999999999998E-4</v>
       </c>
       <c r="C38" s="13">
-        <v>-1.06E-2</v>
+        <v>-5.1999999999999995E-4</v>
       </c>
       <c r="D38" s="13">
         <f t="shared" si="3"/>
-        <v>-1.5900000000000001E-2</v>
+        <v>-7.7999999999999988E-4</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="F38" s="11" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
@@ -1996,26 +1978,26 @@
       </c>
       <c r="B39" s="13">
         <f t="shared" si="2"/>
-        <v>-5.1150000000000001E-2</v>
+        <v>-3.0499999999999999E-4</v>
       </c>
       <c r="C39" s="13">
-        <v>-0.1023</v>
+        <v>-6.0999999999999997E-4</v>
       </c>
       <c r="D39" s="13">
         <f t="shared" si="3"/>
-        <v>-0.15345</v>
+        <v>-9.1500000000000001E-4</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="F39" s="11" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
@@ -2024,26 +2006,26 @@
       </c>
       <c r="B40" s="13">
         <f t="shared" si="2"/>
-        <v>-5.1150000000000001E-2</v>
+        <v>-3.0499999999999999E-4</v>
       </c>
       <c r="C40" s="13">
-        <v>-0.1023</v>
+        <v>-6.0999999999999997E-4</v>
       </c>
       <c r="D40" s="13">
         <f t="shared" si="3"/>
-        <v>-0.15345</v>
+        <v>-9.1500000000000001E-4</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="F40" s="11" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
@@ -2052,305 +2034,295 @@
       </c>
       <c r="B41" s="13">
         <f t="shared" si="2"/>
-        <v>-2.8500000000000001E-3</v>
+        <v>-3.6999999999999999E-4</v>
       </c>
       <c r="C41" s="13">
-        <v>-5.7000000000000002E-3</v>
+        <v>-7.3999999999999999E-4</v>
       </c>
       <c r="D41" s="13">
         <f t="shared" si="3"/>
-        <v>-8.5500000000000003E-3</v>
+        <v>-1.1099999999999999E-3</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="F41" s="11" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B42" s="13">
+        <v>31</v>
+      </c>
+      <c r="B42" s="5">
         <f t="shared" si="2"/>
-        <v>-2.5999999999999998E-4</v>
-      </c>
-      <c r="C42" s="13">
-        <v>-5.1999999999999995E-4</v>
-      </c>
-      <c r="D42" s="13">
+        <v>1.65E-3</v>
+      </c>
+      <c r="C42" s="5">
+        <v>3.3E-3</v>
+      </c>
+      <c r="D42" s="5">
         <f t="shared" si="3"/>
-        <v>-7.7999999999999988E-4</v>
+        <v>4.9499999999999995E-3</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>77</v>
+        <v>41</v>
       </c>
       <c r="F42" s="11" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="H42" s="4" t="s">
-        <v>85</v>
+        <v>116</v>
+      </c>
+      <c r="H42" s="11" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B43" s="13">
+        <v>32</v>
+      </c>
+      <c r="B43" s="5">
         <f t="shared" si="2"/>
-        <v>-2.5999999999999998E-4</v>
-      </c>
-      <c r="C43" s="13">
-        <v>-5.1999999999999995E-4</v>
-      </c>
-      <c r="D43" s="13">
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="C43" s="5">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="D43" s="5">
         <f t="shared" si="3"/>
-        <v>-7.7999999999999988E-4</v>
+        <v>3.7500000000000006E-2</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>77</v>
+        <v>41</v>
       </c>
       <c r="F43" s="11" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="H43" s="4" t="s">
-        <v>85</v>
+        <v>116</v>
+      </c>
+      <c r="H43" s="11" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B44" s="13">
-        <f t="shared" si="2"/>
-        <v>-3.0499999999999999E-4</v>
-      </c>
-      <c r="C44" s="13">
-        <v>-6.0999999999999997E-4</v>
-      </c>
-      <c r="D44" s="13">
-        <f t="shared" si="3"/>
-        <v>-9.1500000000000001E-4</v>
+        <v>33</v>
+      </c>
+      <c r="B44" s="14">
+        <v>0</v>
+      </c>
+      <c r="C44" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="D44" s="14">
+        <v>0.9</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>77</v>
+        <v>41</v>
       </c>
       <c r="F44" s="11" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="H44" s="4" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B45" s="13">
-        <f t="shared" si="2"/>
-        <v>-3.0499999999999999E-4</v>
-      </c>
-      <c r="C45" s="13">
-        <v>-6.0999999999999997E-4</v>
-      </c>
-      <c r="D45" s="13">
-        <f t="shared" si="3"/>
-        <v>-9.1500000000000001E-4</v>
-      </c>
-      <c r="E45" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="F45" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="G45" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="H45" s="4" t="s">
-        <v>85</v>
+        <v>89</v>
+      </c>
+      <c r="H44" s="11" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B45" s="8">
+        <v>0.01</v>
+      </c>
+      <c r="C45" s="8">
+        <v>0.05</v>
+      </c>
+      <c r="D45" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F45" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="G45" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="H45" s="11" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B46" s="13">
-        <f t="shared" si="2"/>
-        <v>-3.6999999999999999E-4</v>
-      </c>
-      <c r="C46" s="13">
-        <v>-7.3999999999999999E-4</v>
-      </c>
-      <c r="D46" s="13">
-        <f t="shared" si="3"/>
-        <v>-1.1099999999999999E-3</v>
-      </c>
-      <c r="E46" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="F46" s="11" t="s">
-        <v>99</v>
+        <v>96</v>
+      </c>
+      <c r="B46" s="15">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="C46" s="15">
+        <v>0.127</v>
+      </c>
+      <c r="D46" s="15">
+        <v>0.23599999999999999</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>94</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="H46" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
+      </c>
+      <c r="H46" s="3" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B47" s="5">
-        <f t="shared" si="2"/>
-        <v>1.65E-3</v>
-      </c>
-      <c r="C47" s="5">
-        <v>3.3E-3</v>
-      </c>
-      <c r="D47" s="5">
-        <f t="shared" si="3"/>
-        <v>4.9499999999999995E-3</v>
-      </c>
-      <c r="E47" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="F47" s="11" t="s">
-        <v>99</v>
+        <v>97</v>
+      </c>
+      <c r="B47" s="15">
+        <v>5.5E-2</v>
+      </c>
+      <c r="C47" s="15">
+        <v>9.8999999999999977E-2</v>
+      </c>
+      <c r="D47" s="15">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>94</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="H47" s="11" t="s">
-        <v>103</v>
+        <v>83</v>
+      </c>
+      <c r="H47" s="3" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B48" s="5">
-        <f t="shared" si="2"/>
-        <v>1.2500000000000001E-2</v>
-      </c>
-      <c r="C48" s="5">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="D48" s="5">
-        <f t="shared" si="3"/>
-        <v>3.7500000000000006E-2</v>
-      </c>
-      <c r="E48" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="F48" s="11" t="s">
-        <v>99</v>
+        <v>98</v>
+      </c>
+      <c r="B48" s="15">
+        <v>5.5E-2</v>
+      </c>
+      <c r="C48" s="15">
+        <v>9.8999999999999977E-2</v>
+      </c>
+      <c r="D48" s="15">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>94</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="H48" s="11" t="s">
-        <v>103</v>
+        <v>83</v>
+      </c>
+      <c r="H48" s="3" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B49" s="14">
-        <v>0</v>
-      </c>
-      <c r="C49" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="D49" s="14">
-        <v>0.9</v>
-      </c>
-      <c r="E49" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="F49" s="11" t="s">
         <v>99</v>
       </c>
+      <c r="B49" s="15">
+        <v>5.5E-2</v>
+      </c>
+      <c r="C49" s="15">
+        <v>9.8999999999999977E-2</v>
+      </c>
+      <c r="D49" s="15">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>94</v>
+      </c>
       <c r="G49" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="H49" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="H49" s="11" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B50" s="8">
-        <v>0.01</v>
-      </c>
-      <c r="C50" s="8">
-        <v>0.05</v>
-      </c>
-      <c r="D50" s="8">
-        <v>0.1</v>
-      </c>
-      <c r="E50" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="F50" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="G50" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="H50" s="11" t="s">
-        <v>104</v>
+      <c r="B50" s="15">
+        <v>5.5E-2</v>
+      </c>
+      <c r="C50" s="15">
+        <v>9.8999999999999977E-2</v>
+      </c>
+      <c r="D50" s="15">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="G50" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="H50" s="3" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B51" s="15">
-        <v>2.1999999999999999E-2</v>
+        <v>8.2000000000000003E-2</v>
       </c>
       <c r="C51" s="15">
-        <v>0.127</v>
+        <v>0.27200000000000002</v>
       </c>
       <c r="D51" s="15">
-        <v>0.23599999999999999</v>
+        <v>0.49399999999999999</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="G51" s="4" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B52" s="15">
         <v>5.5E-2</v>
@@ -2362,21 +2334,21 @@
         <v>0.14299999999999999</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B53" s="15">
         <v>5.5E-2</v>
@@ -2388,21 +2360,21 @@
         <v>0.14299999999999999</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="H53" s="3" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B54" s="15">
         <v>5.5E-2</v>
@@ -2414,125 +2386,125 @@
         <v>0.14299999999999999</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="H54" s="3" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B55" s="15">
-        <v>5.5E-2</v>
+        <v>-1.0999999999999999E-2</v>
       </c>
       <c r="C55" s="15">
-        <v>9.8999999999999977E-2</v>
+        <v>2.8000000000000025E-2</v>
       </c>
       <c r="D55" s="15">
-        <v>0.14299999999999999</v>
+        <v>7.0999999999999994E-2</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="H55" s="3" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
     </row>
     <row r="56" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B56" s="15">
-        <v>8.2000000000000003E-2</v>
+        <v>5.5E-2</v>
       </c>
       <c r="C56" s="15">
-        <v>0.27200000000000002</v>
+        <v>9.8999999999999977E-2</v>
       </c>
       <c r="D56" s="15">
-        <v>0.49399999999999999</v>
+        <v>0.14299999999999999</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="G56" s="4" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="H56" s="3" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
     </row>
     <row r="57" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B57" s="15">
-        <v>5.5E-2</v>
+        <v>1.6E-2</v>
       </c>
       <c r="C57" s="15">
-        <v>9.8999999999999977E-2</v>
+        <v>8.0000000000000071E-2</v>
       </c>
       <c r="D57" s="15">
-        <v>0.14299999999999999</v>
+        <v>0.14799999999999999</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="H57" s="3" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
     </row>
     <row r="58" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B58" s="15">
-        <v>5.5E-2</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="C58" s="15">
         <v>9.8999999999999977E-2</v>
       </c>
       <c r="D58" s="15">
-        <v>0.14299999999999999</v>
+        <v>0.13200000000000001</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="G58" s="4" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="H58" s="3" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
     </row>
     <row r="59" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B59" s="15">
         <v>5.5E-2</v>
@@ -2544,125 +2516,128 @@
         <v>0.14299999999999999</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="G59" s="4" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="H59" s="3" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
     </row>
     <row r="60" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="B60" s="15">
-        <v>-1.0999999999999999E-2</v>
+        <v>5.5E-2</v>
       </c>
       <c r="C60" s="15">
-        <v>2.8000000000000025E-2</v>
+        <v>9.8999999999999977E-2</v>
       </c>
       <c r="D60" s="15">
-        <v>7.0999999999999994E-2</v>
+        <v>0.14299999999999999</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="G60" s="4" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="H60" s="3" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
     </row>
     <row r="61" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B61" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C61" s="15">
+        <v>0.15900000000000003</v>
+      </c>
+      <c r="D61" s="15">
+        <v>0.36299999999999999</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F61" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="G61" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="H61" s="3" t="s">
         <v>117</v>
-      </c>
-      <c r="B61" s="15">
-        <v>5.5E-2</v>
-      </c>
-      <c r="C61" s="15">
-        <v>9.8999999999999977E-2</v>
-      </c>
-      <c r="D61" s="15">
-        <v>0.14299999999999999</v>
-      </c>
-      <c r="E61" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F61" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="G61" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="H61" s="3" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="62" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B62" s="15">
-        <v>1.6E-2</v>
+        <f>B55</f>
+        <v>-1.0999999999999999E-2</v>
       </c>
       <c r="C62" s="15">
-        <v>8.0000000000000071E-2</v>
+        <f t="shared" ref="C62:D62" si="4">C55</f>
+        <v>2.8000000000000025E-2</v>
       </c>
       <c r="D62" s="15">
-        <v>0.14799999999999999</v>
+        <f t="shared" si="4"/>
+        <v>7.0999999999999994E-2</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="G62" s="4" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="H62" s="3" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
     </row>
     <row r="63" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B63" s="15">
-        <v>4.9000000000000002E-2</v>
+        <v>5.5E-2</v>
       </c>
       <c r="C63" s="15">
         <v>9.8999999999999977E-2</v>
       </c>
       <c r="D63" s="15">
-        <v>0.13200000000000001</v>
+        <v>0.14299999999999999</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="G63" s="4" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="H63" s="3" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
     </row>
     <row r="64" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B64" s="15">
         <v>5.5E-2</v>
@@ -2674,21 +2649,21 @@
         <v>0.14299999999999999</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="G64" s="4" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="H64" s="3" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
     </row>
     <row r="65" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B65" s="15">
         <v>5.5E-2</v>
@@ -2700,149 +2675,16 @@
         <v>0.14299999999999999</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="G65" s="4" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="H65" s="3" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="B66" s="15">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="C66" s="15">
-        <v>0.15900000000000003</v>
-      </c>
-      <c r="D66" s="15">
-        <v>0.36299999999999999</v>
-      </c>
-      <c r="E66" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F66" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="G66" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="H66" s="3" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="B67" s="15">
-        <f>B60</f>
-        <v>-1.0999999999999999E-2</v>
-      </c>
-      <c r="C67" s="15">
-        <f t="shared" ref="C67:D67" si="4">C60</f>
-        <v>2.8000000000000025E-2</v>
-      </c>
-      <c r="D67" s="15">
-        <f t="shared" si="4"/>
-        <v>7.0999999999999994E-2</v>
-      </c>
-      <c r="E67" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F67" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="G67" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="H67" s="3" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="B68" s="15">
-        <v>5.5E-2</v>
-      </c>
-      <c r="C68" s="15">
-        <v>9.8999999999999977E-2</v>
-      </c>
-      <c r="D68" s="15">
-        <v>0.14299999999999999</v>
-      </c>
-      <c r="E68" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F68" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="G68" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="H68" s="3" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="B69" s="15">
-        <v>5.5E-2</v>
-      </c>
-      <c r="C69" s="15">
-        <v>9.8999999999999977E-2</v>
-      </c>
-      <c r="D69" s="15">
-        <v>0.14299999999999999</v>
-      </c>
-      <c r="E69" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F69" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="G69" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="H69" s="3" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="B70" s="15">
-        <v>5.5E-2</v>
-      </c>
-      <c r="C70" s="15">
-        <v>9.8999999999999977E-2</v>
-      </c>
-      <c r="D70" s="15">
-        <v>0.14299999999999999</v>
-      </c>
-      <c r="E70" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F70" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="G70" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="H70" s="3" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finished updating parameters in config files
</commit_message>
<xml_diff>
--- a/gcam/input/biochar_land_R/GCAM_parameters.xlsx
+++ b/gcam/input/biochar_land_R/GCAM_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natha\PycharmProjects\IAM\biochar\gcam\input\biochar_land_R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8A341BD-C680-4A01-801F-9DACECAAC689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC76C11A-9BD2-458C-8BFC-9FE8F579ABA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="17385" xr2:uid="{D3FBB104-BEF4-4FDA-A1FA-9751FB33CA85}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{D3FBB104-BEF4-4FDA-A1FA-9751FB33CA85}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="127">
   <si>
     <t>Name</t>
   </si>
@@ -405,6 +405,18 @@
   </si>
   <si>
     <t>Poultry Biochar Net C</t>
+  </si>
+  <si>
+    <t>kg biochar/ha</t>
+  </si>
+  <si>
+    <t>GCAM Model Parameter - all numbers are arbitrary. There's a great deal of near 0 kg/ha application rates, which makes sense for inclusion for agronomic impacts but less sense for the yield increases.</t>
+  </si>
+  <si>
+    <t>Lower limit on application rate to realize biochar yield increase, reduced emissions from land, n fertilizer reduction</t>
+  </si>
+  <si>
+    <t>constants</t>
   </si>
 </sst>
 </file>
@@ -529,7 +541,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -574,6 +586,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="166" fontId="2" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -911,10 +926,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FC7B4C1-BB5E-45EB-9034-E2CB0DD15D7E}">
-  <dimension ref="A1:H65"/>
+  <dimension ref="A1:H66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42:C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2064,7 +2079,7 @@
         <f t="shared" si="2"/>
         <v>1.65E-3</v>
       </c>
-      <c r="C42" s="5">
+      <c r="C42" s="14">
         <v>3.3E-3</v>
       </c>
       <c r="D42" s="5">
@@ -2092,7 +2107,7 @@
         <f t="shared" si="2"/>
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="C43" s="5">
+      <c r="C43" s="14">
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="D43" s="5">
@@ -2119,7 +2134,7 @@
       <c r="B44" s="14">
         <v>0</v>
       </c>
-      <c r="C44" s="5">
+      <c r="C44" s="14">
         <v>0.5</v>
       </c>
       <c r="D44" s="14">
@@ -2164,44 +2179,44 @@
         <v>93</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="B46" s="15">
-        <v>2.1999999999999999E-2</v>
-      </c>
-      <c r="C46" s="15">
-        <v>0.127</v>
-      </c>
-      <c r="D46" s="15">
-        <v>0.23599999999999999</v>
-      </c>
-      <c r="E46" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="F46" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="G46" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="H46" s="3" t="s">
-        <v>117</v>
+    <row r="46" spans="1:8" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="B46" s="16">
+        <v>50</v>
+      </c>
+      <c r="C46" s="16">
+        <v>250</v>
+      </c>
+      <c r="D46" s="16">
+        <v>1000</v>
+      </c>
+      <c r="E46" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="F46" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="G46" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="H46" s="11" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B47" s="15">
-        <v>5.5E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="C47" s="15">
-        <v>9.8999999999999977E-2</v>
+        <v>0.127</v>
       </c>
       <c r="D47" s="15">
-        <v>0.14299999999999999</v>
+        <v>0.23599999999999999</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>41</v>
@@ -2218,7 +2233,7 @@
     </row>
     <row r="48" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B48" s="15">
         <v>5.5E-2</v>
@@ -2244,7 +2259,7 @@
     </row>
     <row r="49" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B49" s="15">
         <v>5.5E-2</v>
@@ -2270,7 +2285,7 @@
     </row>
     <row r="50" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B50" s="15">
         <v>5.5E-2</v>
@@ -2296,16 +2311,16 @@
     </row>
     <row r="51" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B51" s="15">
-        <v>8.2000000000000003E-2</v>
+        <v>5.5E-2</v>
       </c>
       <c r="C51" s="15">
-        <v>0.27200000000000002</v>
+        <v>9.8999999999999977E-2</v>
       </c>
       <c r="D51" s="15">
-        <v>0.49399999999999999</v>
+        <v>0.14299999999999999</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>41</v>
@@ -2322,16 +2337,16 @@
     </row>
     <row r="52" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B52" s="15">
-        <v>5.5E-2</v>
+        <v>8.2000000000000003E-2</v>
       </c>
       <c r="C52" s="15">
-        <v>9.8999999999999977E-2</v>
+        <v>0.27200000000000002</v>
       </c>
       <c r="D52" s="15">
-        <v>0.14299999999999999</v>
+        <v>0.49399999999999999</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>41</v>
@@ -2348,7 +2363,7 @@
     </row>
     <row r="53" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B53" s="15">
         <v>5.5E-2</v>
@@ -2374,7 +2389,7 @@
     </row>
     <row r="54" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B54" s="15">
         <v>5.5E-2</v>
@@ -2400,16 +2415,16 @@
     </row>
     <row r="55" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B55" s="15">
-        <v>-1.0999999999999999E-2</v>
+        <v>5.5E-2</v>
       </c>
       <c r="C55" s="15">
-        <v>2.8000000000000025E-2</v>
+        <v>9.8999999999999977E-2</v>
       </c>
       <c r="D55" s="15">
-        <v>7.0999999999999994E-2</v>
+        <v>0.14299999999999999</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>41</v>
@@ -2426,16 +2441,16 @@
     </row>
     <row r="56" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B56" s="15">
-        <v>5.5E-2</v>
+        <v>-1.0999999999999999E-2</v>
       </c>
       <c r="C56" s="15">
-        <v>9.8999999999999977E-2</v>
+        <v>2.8000000000000025E-2</v>
       </c>
       <c r="D56" s="15">
-        <v>0.14299999999999999</v>
+        <v>7.0999999999999994E-2</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>41</v>
@@ -2452,16 +2467,16 @@
     </row>
     <row r="57" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B57" s="15">
-        <v>1.6E-2</v>
+        <v>5.5E-2</v>
       </c>
       <c r="C57" s="15">
-        <v>8.0000000000000071E-2</v>
+        <v>9.8999999999999977E-2</v>
       </c>
       <c r="D57" s="15">
-        <v>0.14799999999999999</v>
+        <v>0.14299999999999999</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>41</v>
@@ -2478,16 +2493,16 @@
     </row>
     <row r="58" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B58" s="15">
-        <v>4.9000000000000002E-2</v>
+        <v>1.6E-2</v>
       </c>
       <c r="C58" s="15">
-        <v>9.8999999999999977E-2</v>
+        <v>8.0000000000000071E-2</v>
       </c>
       <c r="D58" s="15">
-        <v>0.13200000000000001</v>
+        <v>0.14799999999999999</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>41</v>
@@ -2504,16 +2519,16 @@
     </row>
     <row r="59" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B59" s="15">
-        <v>5.5E-2</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="C59" s="15">
         <v>9.8999999999999977E-2</v>
       </c>
       <c r="D59" s="15">
-        <v>0.14299999999999999</v>
+        <v>0.13200000000000001</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>41</v>
@@ -2530,7 +2545,7 @@
     </row>
     <row r="60" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B60" s="15">
         <v>5.5E-2</v>
@@ -2556,16 +2571,16 @@
     </row>
     <row r="61" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B61" s="15">
-        <v>5.0000000000000001E-3</v>
+        <v>5.5E-2</v>
       </c>
       <c r="C61" s="15">
-        <v>0.15900000000000003</v>
+        <v>9.8999999999999977E-2</v>
       </c>
       <c r="D61" s="15">
-        <v>0.36299999999999999</v>
+        <v>0.14299999999999999</v>
       </c>
       <c r="E61" s="3" t="s">
         <v>41</v>
@@ -2582,46 +2597,46 @@
     </row>
     <row r="62" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B62" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C62" s="15">
+        <v>0.15900000000000003</v>
+      </c>
+      <c r="D62" s="15">
+        <v>0.36299999999999999</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F62" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="G62" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="H62" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="B62" s="15">
-        <f>B55</f>
+      <c r="B63" s="15">
+        <f>B56</f>
         <v>-1.0999999999999999E-2</v>
       </c>
-      <c r="C62" s="15">
-        <f t="shared" ref="C62:D62" si="4">C55</f>
+      <c r="C63" s="15">
+        <f t="shared" ref="C63:D63" si="4">C56</f>
         <v>2.8000000000000025E-2</v>
       </c>
-      <c r="D62" s="15">
+      <c r="D63" s="15">
         <f t="shared" si="4"/>
         <v>7.0999999999999994E-2</v>
       </c>
-      <c r="E62" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="F62" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="G62" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="H62" s="3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="B63" s="15">
-        <v>5.5E-2</v>
-      </c>
-      <c r="C63" s="15">
-        <v>9.8999999999999977E-2</v>
-      </c>
-      <c r="D63" s="15">
-        <v>0.14299999999999999</v>
-      </c>
       <c r="E63" s="3" t="s">
         <v>41</v>
       </c>
@@ -2637,7 +2652,7 @@
     </row>
     <row r="64" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B64" s="15">
         <v>5.5E-2</v>
@@ -2663,7 +2678,7 @@
     </row>
     <row r="65" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B65" s="15">
         <v>5.5E-2</v>
@@ -2684,6 +2699,32 @@
         <v>83</v>
       </c>
       <c r="H65" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B66" s="15">
+        <v>5.5E-2</v>
+      </c>
+      <c r="C66" s="15">
+        <v>9.8999999999999977E-2</v>
+      </c>
+      <c r="D66" s="15">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F66" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="G66" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="H66" s="3" t="s">
         <v>117</v>
       </c>
     </row>

</xml_diff>

<commit_message>
sensitivity analysis config files
</commit_message>
<xml_diff>
--- a/gcam/input/biochar_land_R/GCAM_parameters.xlsx
+++ b/gcam/input/biochar_land_R/GCAM_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natha\PycharmProjects\IAM\biochar\gcam\input\biochar_land_R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC76C11A-9BD2-458C-8BFC-9FE8F579ABA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFA02CED-6C28-467A-B742-891117C378A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{D3FBB104-BEF4-4FDA-A1FA-9751FB33CA85}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="17385" xr2:uid="{D3FBB104-BEF4-4FDA-A1FA-9751FB33CA85}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -541,7 +541,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -576,9 +576,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -589,6 +586,12 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -928,8 +931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FC7B4C1-BB5E-45EB-9034-E2CB0DD15D7E}">
   <dimension ref="A1:H66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42:C44"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1652,27 +1655,27 @@
       </c>
     </row>
     <row r="27" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="6" t="s">
+      <c r="A27" s="16" t="s">
         <v>118</v>
       </c>
-      <c r="B27" s="12">
+      <c r="B27" s="17">
         <f>0.5*C27</f>
         <v>-0.125</v>
       </c>
-      <c r="C27" s="12">
+      <c r="C27" s="17">
         <v>-0.25</v>
       </c>
-      <c r="D27" s="12">
+      <c r="D27" s="17">
         <f>1.5*C27</f>
         <v>-0.375</v>
       </c>
-      <c r="E27" s="7" t="s">
+      <c r="E27" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="F27" s="7" t="s">
+      <c r="F27" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="G27" s="7" t="s">
+      <c r="G27" s="11" t="s">
         <v>116</v>
       </c>
       <c r="H27" s="4" t="s">
@@ -1680,27 +1683,27 @@
       </c>
     </row>
     <row r="28" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="6" t="s">
+      <c r="A28" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="B28" s="12">
+      <c r="B28" s="17">
         <f t="shared" ref="B28:B43" si="2">0.5*C28</f>
         <v>-0.125</v>
       </c>
-      <c r="C28" s="12">
+      <c r="C28" s="17">
         <v>-0.25</v>
       </c>
-      <c r="D28" s="12">
+      <c r="D28" s="17">
         <f t="shared" ref="D28:D43" si="3">1.5*C28</f>
         <v>-0.375</v>
       </c>
-      <c r="E28" s="7" t="s">
+      <c r="E28" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="F28" s="7" t="s">
+      <c r="F28" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="G28" s="7" t="s">
+      <c r="G28" s="11" t="s">
         <v>116</v>
       </c>
       <c r="H28" s="4" t="s">
@@ -1708,27 +1711,27 @@
       </c>
     </row>
     <row r="29" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="6" t="s">
+      <c r="A29" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="B29" s="12">
+      <c r="B29" s="17">
         <f t="shared" si="2"/>
         <v>-0.155</v>
       </c>
-      <c r="C29" s="12">
+      <c r="C29" s="17">
         <v>-0.31</v>
       </c>
-      <c r="D29" s="12">
+      <c r="D29" s="17">
         <f t="shared" si="3"/>
         <v>-0.46499999999999997</v>
       </c>
-      <c r="E29" s="7" t="s">
+      <c r="E29" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="F29" s="7" t="s">
+      <c r="F29" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="G29" s="7" t="s">
+      <c r="G29" s="11" t="s">
         <v>116</v>
       </c>
       <c r="H29" s="4" t="s">
@@ -1736,27 +1739,27 @@
       </c>
     </row>
     <row r="30" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="6" t="s">
+      <c r="A30" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="B30" s="12">
+      <c r="B30" s="17">
         <f t="shared" si="2"/>
         <v>-0.155</v>
       </c>
-      <c r="C30" s="12">
+      <c r="C30" s="17">
         <v>-0.31</v>
       </c>
-      <c r="D30" s="12">
+      <c r="D30" s="17">
         <f t="shared" si="3"/>
         <v>-0.46499999999999997</v>
       </c>
-      <c r="E30" s="7" t="s">
+      <c r="E30" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="F30" s="7" t="s">
+      <c r="F30" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="G30" s="7" t="s">
+      <c r="G30" s="11" t="s">
         <v>116</v>
       </c>
       <c r="H30" s="4" t="s">
@@ -1764,27 +1767,27 @@
       </c>
     </row>
     <row r="31" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="6" t="s">
+      <c r="A31" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="B31" s="12">
+      <c r="B31" s="17">
         <f t="shared" si="2"/>
         <v>-0.14000000000000001</v>
       </c>
-      <c r="C31" s="12">
+      <c r="C31" s="17">
         <v>-0.28000000000000003</v>
       </c>
-      <c r="D31" s="12">
+      <c r="D31" s="17">
         <f t="shared" si="3"/>
         <v>-0.42000000000000004</v>
       </c>
-      <c r="E31" s="7" t="s">
+      <c r="E31" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="F31" s="7" t="s">
+      <c r="F31" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="G31" s="7" t="s">
+      <c r="G31" s="11" t="s">
         <v>116</v>
       </c>
       <c r="H31" s="4" t="s">
@@ -1795,14 +1798,14 @@
       <c r="A32" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B32" s="13">
+      <c r="B32" s="12">
         <f t="shared" si="2"/>
         <v>-5.3E-3</v>
       </c>
-      <c r="C32" s="13">
+      <c r="C32" s="12">
         <v>-1.06E-2</v>
       </c>
-      <c r="D32" s="13">
+      <c r="D32" s="12">
         <f t="shared" si="3"/>
         <v>-1.5900000000000001E-2</v>
       </c>
@@ -1823,14 +1826,14 @@
       <c r="A33" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B33" s="13">
+      <c r="B33" s="12">
         <f t="shared" si="2"/>
         <v>-5.3E-3</v>
       </c>
-      <c r="C33" s="13">
+      <c r="C33" s="12">
         <v>-1.06E-2</v>
       </c>
-      <c r="D33" s="13">
+      <c r="D33" s="12">
         <f t="shared" si="3"/>
         <v>-1.5900000000000001E-2</v>
       </c>
@@ -1851,14 +1854,14 @@
       <c r="A34" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B34" s="13">
+      <c r="B34" s="12">
         <f t="shared" si="2"/>
         <v>-5.1150000000000001E-2</v>
       </c>
-      <c r="C34" s="13">
+      <c r="C34" s="12">
         <v>-0.1023</v>
       </c>
-      <c r="D34" s="13">
+      <c r="D34" s="12">
         <f t="shared" si="3"/>
         <v>-0.15345</v>
       </c>
@@ -1879,14 +1882,14 @@
       <c r="A35" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B35" s="13">
+      <c r="B35" s="12">
         <f t="shared" si="2"/>
         <v>-5.1150000000000001E-2</v>
       </c>
-      <c r="C35" s="13">
+      <c r="C35" s="12">
         <v>-0.1023</v>
       </c>
-      <c r="D35" s="13">
+      <c r="D35" s="12">
         <f t="shared" si="3"/>
         <v>-0.15345</v>
       </c>
@@ -1907,14 +1910,14 @@
       <c r="A36" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B36" s="13">
+      <c r="B36" s="12">
         <f t="shared" si="2"/>
         <v>-2.8500000000000001E-3</v>
       </c>
-      <c r="C36" s="13">
+      <c r="C36" s="12">
         <v>-5.7000000000000002E-3</v>
       </c>
-      <c r="D36" s="13">
+      <c r="D36" s="12">
         <f t="shared" si="3"/>
         <v>-8.5500000000000003E-3</v>
       </c>
@@ -1935,14 +1938,14 @@
       <c r="A37" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B37" s="13">
+      <c r="B37" s="12">
         <f t="shared" si="2"/>
         <v>-2.5999999999999998E-4</v>
       </c>
-      <c r="C37" s="13">
+      <c r="C37" s="12">
         <v>-5.1999999999999995E-4</v>
       </c>
-      <c r="D37" s="13">
+      <c r="D37" s="12">
         <f t="shared" si="3"/>
         <v>-7.7999999999999988E-4</v>
       </c>
@@ -1963,14 +1966,14 @@
       <c r="A38" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B38" s="13">
+      <c r="B38" s="12">
         <f t="shared" si="2"/>
         <v>-2.5999999999999998E-4</v>
       </c>
-      <c r="C38" s="13">
+      <c r="C38" s="12">
         <v>-5.1999999999999995E-4</v>
       </c>
-      <c r="D38" s="13">
+      <c r="D38" s="12">
         <f t="shared" si="3"/>
         <v>-7.7999999999999988E-4</v>
       </c>
@@ -1991,14 +1994,14 @@
       <c r="A39" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B39" s="13">
+      <c r="B39" s="12">
         <f t="shared" si="2"/>
         <v>-3.0499999999999999E-4</v>
       </c>
-      <c r="C39" s="13">
+      <c r="C39" s="12">
         <v>-6.0999999999999997E-4</v>
       </c>
-      <c r="D39" s="13">
+      <c r="D39" s="12">
         <f t="shared" si="3"/>
         <v>-9.1500000000000001E-4</v>
       </c>
@@ -2019,14 +2022,14 @@
       <c r="A40" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B40" s="13">
+      <c r="B40" s="12">
         <f t="shared" si="2"/>
         <v>-3.0499999999999999E-4</v>
       </c>
-      <c r="C40" s="13">
+      <c r="C40" s="12">
         <v>-6.0999999999999997E-4</v>
       </c>
-      <c r="D40" s="13">
+      <c r="D40" s="12">
         <f t="shared" si="3"/>
         <v>-9.1500000000000001E-4</v>
       </c>
@@ -2047,14 +2050,14 @@
       <c r="A41" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B41" s="13">
+      <c r="B41" s="12">
         <f t="shared" si="2"/>
         <v>-3.6999999999999999E-4</v>
       </c>
-      <c r="C41" s="13">
+      <c r="C41" s="12">
         <v>-7.3999999999999999E-4</v>
       </c>
-      <c r="D41" s="13">
+      <c r="D41" s="12">
         <f t="shared" si="3"/>
         <v>-1.1099999999999999E-3</v>
       </c>
@@ -2079,7 +2082,7 @@
         <f t="shared" si="2"/>
         <v>1.65E-3</v>
       </c>
-      <c r="C42" s="14">
+      <c r="C42" s="13">
         <v>3.3E-3</v>
       </c>
       <c r="D42" s="5">
@@ -2107,7 +2110,7 @@
         <f t="shared" si="2"/>
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="C43" s="14">
+      <c r="C43" s="13">
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="D43" s="5">
@@ -2131,13 +2134,13 @@
       <c r="A44" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B44" s="14">
+      <c r="B44" s="13">
         <v>0</v>
       </c>
-      <c r="C44" s="14">
+      <c r="C44" s="13">
         <v>0.5</v>
       </c>
-      <c r="D44" s="14">
+      <c r="D44" s="13">
         <v>0.9</v>
       </c>
       <c r="E44" s="4" t="s">
@@ -2183,13 +2186,13 @@
       <c r="A46" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="B46" s="16">
+      <c r="B46" s="15">
         <v>50</v>
       </c>
-      <c r="C46" s="16">
+      <c r="C46" s="15">
         <v>250</v>
       </c>
-      <c r="D46" s="16">
+      <c r="D46" s="15">
         <v>1000</v>
       </c>
       <c r="E46" s="7" t="s">
@@ -2209,13 +2212,13 @@
       <c r="A47" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B47" s="15">
+      <c r="B47" s="14">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="C47" s="15">
+      <c r="C47" s="14">
         <v>0.127</v>
       </c>
-      <c r="D47" s="15">
+      <c r="D47" s="14">
         <v>0.23599999999999999</v>
       </c>
       <c r="E47" s="3" t="s">
@@ -2235,13 +2238,13 @@
       <c r="A48" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B48" s="15">
+      <c r="B48" s="14">
         <v>5.5E-2</v>
       </c>
-      <c r="C48" s="15">
+      <c r="C48" s="14">
         <v>9.8999999999999977E-2</v>
       </c>
-      <c r="D48" s="15">
+      <c r="D48" s="14">
         <v>0.14299999999999999</v>
       </c>
       <c r="E48" s="3" t="s">
@@ -2261,13 +2264,13 @@
       <c r="A49" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B49" s="15">
+      <c r="B49" s="14">
         <v>5.5E-2</v>
       </c>
-      <c r="C49" s="15">
+      <c r="C49" s="14">
         <v>9.8999999999999977E-2</v>
       </c>
-      <c r="D49" s="15">
+      <c r="D49" s="14">
         <v>0.14299999999999999</v>
       </c>
       <c r="E49" s="3" t="s">
@@ -2287,13 +2290,13 @@
       <c r="A50" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B50" s="15">
+      <c r="B50" s="14">
         <v>5.5E-2</v>
       </c>
-      <c r="C50" s="15">
+      <c r="C50" s="14">
         <v>9.8999999999999977E-2</v>
       </c>
-      <c r="D50" s="15">
+      <c r="D50" s="14">
         <v>0.14299999999999999</v>
       </c>
       <c r="E50" s="3" t="s">
@@ -2313,13 +2316,13 @@
       <c r="A51" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B51" s="15">
+      <c r="B51" s="14">
         <v>5.5E-2</v>
       </c>
-      <c r="C51" s="15">
+      <c r="C51" s="14">
         <v>9.8999999999999977E-2</v>
       </c>
-      <c r="D51" s="15">
+      <c r="D51" s="14">
         <v>0.14299999999999999</v>
       </c>
       <c r="E51" s="3" t="s">
@@ -2339,13 +2342,13 @@
       <c r="A52" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="B52" s="15">
+      <c r="B52" s="14">
         <v>8.2000000000000003E-2</v>
       </c>
-      <c r="C52" s="15">
+      <c r="C52" s="14">
         <v>0.27200000000000002</v>
       </c>
-      <c r="D52" s="15">
+      <c r="D52" s="14">
         <v>0.49399999999999999</v>
       </c>
       <c r="E52" s="3" t="s">
@@ -2365,13 +2368,13 @@
       <c r="A53" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B53" s="15">
+      <c r="B53" s="14">
         <v>5.5E-2</v>
       </c>
-      <c r="C53" s="15">
+      <c r="C53" s="14">
         <v>9.8999999999999977E-2</v>
       </c>
-      <c r="D53" s="15">
+      <c r="D53" s="14">
         <v>0.14299999999999999</v>
       </c>
       <c r="E53" s="3" t="s">
@@ -2391,13 +2394,13 @@
       <c r="A54" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B54" s="15">
+      <c r="B54" s="14">
         <v>5.5E-2</v>
       </c>
-      <c r="C54" s="15">
+      <c r="C54" s="14">
         <v>9.8999999999999977E-2</v>
       </c>
-      <c r="D54" s="15">
+      <c r="D54" s="14">
         <v>0.14299999999999999</v>
       </c>
       <c r="E54" s="3" t="s">
@@ -2417,13 +2420,13 @@
       <c r="A55" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B55" s="15">
+      <c r="B55" s="14">
         <v>5.5E-2</v>
       </c>
-      <c r="C55" s="15">
+      <c r="C55" s="14">
         <v>9.8999999999999977E-2</v>
       </c>
-      <c r="D55" s="15">
+      <c r="D55" s="14">
         <v>0.14299999999999999</v>
       </c>
       <c r="E55" s="3" t="s">
@@ -2443,13 +2446,13 @@
       <c r="A56" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="B56" s="15">
+      <c r="B56" s="14">
         <v>-1.0999999999999999E-2</v>
       </c>
-      <c r="C56" s="15">
+      <c r="C56" s="14">
         <v>2.8000000000000025E-2</v>
       </c>
-      <c r="D56" s="15">
+      <c r="D56" s="14">
         <v>7.0999999999999994E-2</v>
       </c>
       <c r="E56" s="3" t="s">
@@ -2469,13 +2472,13 @@
       <c r="A57" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="B57" s="15">
+      <c r="B57" s="14">
         <v>5.5E-2</v>
       </c>
-      <c r="C57" s="15">
+      <c r="C57" s="14">
         <v>9.8999999999999977E-2</v>
       </c>
-      <c r="D57" s="15">
+      <c r="D57" s="14">
         <v>0.14299999999999999</v>
       </c>
       <c r="E57" s="3" t="s">
@@ -2495,13 +2498,13 @@
       <c r="A58" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="B58" s="15">
+      <c r="B58" s="14">
         <v>1.6E-2</v>
       </c>
-      <c r="C58" s="15">
+      <c r="C58" s="14">
         <v>8.0000000000000071E-2</v>
       </c>
-      <c r="D58" s="15">
+      <c r="D58" s="14">
         <v>0.14799999999999999</v>
       </c>
       <c r="E58" s="3" t="s">
@@ -2521,13 +2524,13 @@
       <c r="A59" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="B59" s="15">
+      <c r="B59" s="14">
         <v>4.9000000000000002E-2</v>
       </c>
-      <c r="C59" s="15">
+      <c r="C59" s="14">
         <v>9.8999999999999977E-2</v>
       </c>
-      <c r="D59" s="15">
+      <c r="D59" s="14">
         <v>0.13200000000000001</v>
       </c>
       <c r="E59" s="3" t="s">
@@ -2547,13 +2550,13 @@
       <c r="A60" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="B60" s="15">
+      <c r="B60" s="14">
         <v>5.5E-2</v>
       </c>
-      <c r="C60" s="15">
+      <c r="C60" s="14">
         <v>9.8999999999999977E-2</v>
       </c>
-      <c r="D60" s="15">
+      <c r="D60" s="14">
         <v>0.14299999999999999</v>
       </c>
       <c r="E60" s="3" t="s">
@@ -2573,13 +2576,13 @@
       <c r="A61" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B61" s="15">
+      <c r="B61" s="14">
         <v>5.5E-2</v>
       </c>
-      <c r="C61" s="15">
+      <c r="C61" s="14">
         <v>9.8999999999999977E-2</v>
       </c>
-      <c r="D61" s="15">
+      <c r="D61" s="14">
         <v>0.14299999999999999</v>
       </c>
       <c r="E61" s="3" t="s">
@@ -2599,13 +2602,13 @@
       <c r="A62" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="B62" s="15">
+      <c r="B62" s="14">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="C62" s="15">
+      <c r="C62" s="14">
         <v>0.15900000000000003</v>
       </c>
-      <c r="D62" s="15">
+      <c r="D62" s="14">
         <v>0.36299999999999999</v>
       </c>
       <c r="E62" s="3" t="s">
@@ -2625,15 +2628,15 @@
       <c r="A63" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="B63" s="15">
+      <c r="B63" s="14">
         <f>B56</f>
         <v>-1.0999999999999999E-2</v>
       </c>
-      <c r="C63" s="15">
+      <c r="C63" s="14">
         <f t="shared" ref="C63:D63" si="4">C56</f>
         <v>2.8000000000000025E-2</v>
       </c>
-      <c r="D63" s="15">
+      <c r="D63" s="14">
         <f t="shared" si="4"/>
         <v>7.0999999999999994E-2</v>
       </c>
@@ -2654,13 +2657,13 @@
       <c r="A64" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="B64" s="15">
+      <c r="B64" s="14">
         <v>5.5E-2</v>
       </c>
-      <c r="C64" s="15">
+      <c r="C64" s="14">
         <v>9.8999999999999977E-2</v>
       </c>
-      <c r="D64" s="15">
+      <c r="D64" s="14">
         <v>0.14299999999999999</v>
       </c>
       <c r="E64" s="3" t="s">
@@ -2680,13 +2683,13 @@
       <c r="A65" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="B65" s="15">
+      <c r="B65" s="14">
         <v>5.5E-2</v>
       </c>
-      <c r="C65" s="15">
+      <c r="C65" s="14">
         <v>9.8999999999999977E-2</v>
       </c>
-      <c r="D65" s="15">
+      <c r="D65" s="14">
         <v>0.14299999999999999</v>
       </c>
       <c r="E65" s="3" t="s">
@@ -2706,13 +2709,13 @@
       <c r="A66" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="B66" s="15">
+      <c r="B66" s="14">
         <v>5.5E-2</v>
       </c>
-      <c r="C66" s="15">
+      <c r="C66" s="14">
         <v>9.8999999999999977E-2</v>
       </c>
-      <c r="D66" s="15">
+      <c r="D66" s="14">
         <v>0.14299999999999999</v>
       </c>
       <c r="E66" s="3" t="s">

</xml_diff>

<commit_message>
modified parameters to ensure model output for debugging
</commit_message>
<xml_diff>
--- a/gcam/input/biochar_land_R/GCAM_parameters.xlsx
+++ b/gcam/input/biochar_land_R/GCAM_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natha\PycharmProjects\IAM\biochar\gcam\input\biochar_land_R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFA02CED-6C28-467A-B742-891117C378A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63B9ACDD-55F5-4DD8-AE77-E00F0604859A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="17385" xr2:uid="{D3FBB104-BEF4-4FDA-A1FA-9751FB33CA85}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{D3FBB104-BEF4-4FDA-A1FA-9751FB33CA85}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -931,8 +931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FC7B4C1-BB5E-45EB-9034-E2CB0DD15D7E}">
   <dimension ref="A1:H66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2187,13 +2187,13 @@
         <v>125</v>
       </c>
       <c r="B46" s="15">
-        <v>50</v>
+        <v>250</v>
       </c>
       <c r="C46" s="15">
-        <v>250</v>
+        <v>1000</v>
       </c>
       <c r="D46" s="15">
-        <v>1000</v>
+        <v>2500</v>
       </c>
       <c r="E46" s="7" t="s">
         <v>123</v>

</xml_diff>

<commit_message>
biochar yield sensitivity analysis update
</commit_message>
<xml_diff>
--- a/gcam/input/biochar_land_R/GCAM_parameters.xlsx
+++ b/gcam/input/biochar_land_R/GCAM_parameters.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natha\PycharmProjects\IAM\biochar\gcam\input\biochar_land_R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63B9ACDD-55F5-4DD8-AE77-E00F0604859A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D01F8A64-D62F-4CA1-AD07-E7B48831D201}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{D3FBB104-BEF4-4FDA-A1FA-9751FB33CA85}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{D3FBB104-BEF4-4FDA-A1FA-9751FB33CA85}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="138">
   <si>
     <t>Name</t>
   </si>
@@ -417,6 +418,39 @@
   </si>
   <si>
     <t>constants</t>
+  </si>
+  <si>
+    <t>Scenario tracker</t>
+  </si>
+  <si>
+    <t>6p0</t>
+  </si>
+  <si>
+    <t>2p6</t>
+  </si>
+  <si>
+    <t>Default</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>BiocharYieldHigh</t>
+  </si>
+  <si>
+    <t>running</t>
+  </si>
+  <si>
+    <t>BiocharYieldLow</t>
+  </si>
+  <si>
+    <t>NutrientYieldLow</t>
+  </si>
+  <si>
+    <t>NutrientYieldHigh</t>
   </si>
 </sst>
 </file>
@@ -570,9 +604,6 @@
     <xf numFmtId="10" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="2" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -585,13 +616,16 @@
     <xf numFmtId="166" fontId="2" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -931,8 +965,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FC7B4C1-BB5E-45EB-9034-E2CB0DD15D7E}">
   <dimension ref="A1:H66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView topLeftCell="A15" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1164,7 +1198,7 @@
       <c r="G8" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="H8" s="11" t="s">
+      <c r="H8" s="10" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1192,7 +1226,7 @@
       <c r="G9" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="H9" s="11" t="s">
+      <c r="H9" s="10" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1249,7 +1283,7 @@
       <c r="G11" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="H11" s="11" t="s">
+      <c r="H11" s="10" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1278,7 +1312,7 @@
       <c r="G12" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="H12" s="11" t="s">
+      <c r="H12" s="10" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1316,7 +1350,7 @@
         <f>C14*0.5</f>
         <v>1.75E-3</v>
       </c>
-      <c r="C14" s="10">
+      <c r="C14" s="9">
         <v>3.5000000000000001E-3</v>
       </c>
       <c r="D14" s="9">
@@ -1332,7 +1366,7 @@
       <c r="G14" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="H14" s="11" t="s">
+      <c r="H14" s="10" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1344,7 +1378,7 @@
         <f>C15*0.5</f>
         <v>1.4E-2</v>
       </c>
-      <c r="C15" s="10">
+      <c r="C15" s="9">
         <v>2.8000000000000001E-2</v>
       </c>
       <c r="D15" s="9">
@@ -1360,7 +1394,7 @@
       <c r="G15" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="H15" s="11" t="s">
+      <c r="H15" s="10" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1412,7 +1446,7 @@
       <c r="G17" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="H17" s="11" t="s">
+      <c r="H17" s="10" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1438,7 +1472,7 @@
       <c r="G18" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="H18" s="11" t="s">
+      <c r="H18" s="10" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1492,7 +1526,7 @@
       <c r="G20" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="H20" s="11" t="s">
+      <c r="H20" s="10" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1520,7 +1554,7 @@
       <c r="G21" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="H21" s="11" t="s">
+      <c r="H21" s="10" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1655,27 +1689,27 @@
       </c>
     </row>
     <row r="27" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="16" t="s">
+      <c r="A27" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="B27" s="17">
+      <c r="B27" s="15">
         <f>0.5*C27</f>
         <v>-0.125</v>
       </c>
-      <c r="C27" s="17">
+      <c r="C27" s="15">
         <v>-0.25</v>
       </c>
-      <c r="D27" s="17">
+      <c r="D27" s="15">
         <f>1.5*C27</f>
         <v>-0.375</v>
       </c>
-      <c r="E27" s="11" t="s">
+      <c r="E27" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="F27" s="11" t="s">
+      <c r="F27" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="G27" s="11" t="s">
+      <c r="G27" s="10" t="s">
         <v>116</v>
       </c>
       <c r="H27" s="4" t="s">
@@ -1683,27 +1717,27 @@
       </c>
     </row>
     <row r="28" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="16" t="s">
+      <c r="A28" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="B28" s="17">
+      <c r="B28" s="15">
         <f t="shared" ref="B28:B43" si="2">0.5*C28</f>
         <v>-0.125</v>
       </c>
-      <c r="C28" s="17">
+      <c r="C28" s="15">
         <v>-0.25</v>
       </c>
-      <c r="D28" s="17">
+      <c r="D28" s="15">
         <f t="shared" ref="D28:D43" si="3">1.5*C28</f>
         <v>-0.375</v>
       </c>
-      <c r="E28" s="11" t="s">
+      <c r="E28" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="F28" s="11" t="s">
+      <c r="F28" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="G28" s="11" t="s">
+      <c r="G28" s="10" t="s">
         <v>116</v>
       </c>
       <c r="H28" s="4" t="s">
@@ -1711,27 +1745,27 @@
       </c>
     </row>
     <row r="29" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="16" t="s">
+      <c r="A29" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="B29" s="17">
+      <c r="B29" s="15">
         <f t="shared" si="2"/>
         <v>-0.155</v>
       </c>
-      <c r="C29" s="17">
+      <c r="C29" s="15">
         <v>-0.31</v>
       </c>
-      <c r="D29" s="17">
+      <c r="D29" s="15">
         <f t="shared" si="3"/>
         <v>-0.46499999999999997</v>
       </c>
-      <c r="E29" s="11" t="s">
+      <c r="E29" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="F29" s="11" t="s">
+      <c r="F29" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="G29" s="11" t="s">
+      <c r="G29" s="10" t="s">
         <v>116</v>
       </c>
       <c r="H29" s="4" t="s">
@@ -1739,27 +1773,27 @@
       </c>
     </row>
     <row r="30" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="16" t="s">
+      <c r="A30" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="B30" s="17">
+      <c r="B30" s="15">
         <f t="shared" si="2"/>
         <v>-0.155</v>
       </c>
-      <c r="C30" s="17">
+      <c r="C30" s="15">
         <v>-0.31</v>
       </c>
-      <c r="D30" s="17">
+      <c r="D30" s="15">
         <f t="shared" si="3"/>
         <v>-0.46499999999999997</v>
       </c>
-      <c r="E30" s="11" t="s">
+      <c r="E30" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="F30" s="11" t="s">
+      <c r="F30" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="G30" s="11" t="s">
+      <c r="G30" s="10" t="s">
         <v>116</v>
       </c>
       <c r="H30" s="4" t="s">
@@ -1767,27 +1801,27 @@
       </c>
     </row>
     <row r="31" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="16" t="s">
+      <c r="A31" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="B31" s="17">
+      <c r="B31" s="15">
         <f t="shared" si="2"/>
         <v>-0.14000000000000001</v>
       </c>
-      <c r="C31" s="17">
+      <c r="C31" s="15">
         <v>-0.28000000000000003</v>
       </c>
-      <c r="D31" s="17">
+      <c r="D31" s="15">
         <f t="shared" si="3"/>
         <v>-0.42000000000000004</v>
       </c>
-      <c r="E31" s="11" t="s">
+      <c r="E31" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="F31" s="11" t="s">
+      <c r="F31" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="G31" s="11" t="s">
+      <c r="G31" s="10" t="s">
         <v>116</v>
       </c>
       <c r="H31" s="4" t="s">
@@ -1798,21 +1832,21 @@
       <c r="A32" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B32" s="12">
+      <c r="B32" s="11">
         <f t="shared" si="2"/>
         <v>-5.3E-3</v>
       </c>
-      <c r="C32" s="12">
+      <c r="C32" s="11">
         <v>-1.06E-2</v>
       </c>
-      <c r="D32" s="12">
+      <c r="D32" s="11">
         <f t="shared" si="3"/>
         <v>-1.5900000000000001E-2</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="F32" s="11" t="s">
+      <c r="F32" s="10" t="s">
         <v>88</v>
       </c>
       <c r="G32" s="4" t="s">
@@ -1826,21 +1860,21 @@
       <c r="A33" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B33" s="12">
+      <c r="B33" s="11">
         <f t="shared" si="2"/>
         <v>-5.3E-3</v>
       </c>
-      <c r="C33" s="12">
+      <c r="C33" s="11">
         <v>-1.06E-2</v>
       </c>
-      <c r="D33" s="12">
+      <c r="D33" s="11">
         <f t="shared" si="3"/>
         <v>-1.5900000000000001E-2</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="F33" s="11" t="s">
+      <c r="F33" s="10" t="s">
         <v>88</v>
       </c>
       <c r="G33" s="4" t="s">
@@ -1854,21 +1888,21 @@
       <c r="A34" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B34" s="12">
+      <c r="B34" s="11">
         <f t="shared" si="2"/>
         <v>-5.1150000000000001E-2</v>
       </c>
-      <c r="C34" s="12">
+      <c r="C34" s="11">
         <v>-0.1023</v>
       </c>
-      <c r="D34" s="12">
+      <c r="D34" s="11">
         <f t="shared" si="3"/>
         <v>-0.15345</v>
       </c>
       <c r="E34" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="F34" s="11" t="s">
+      <c r="F34" s="10" t="s">
         <v>88</v>
       </c>
       <c r="G34" s="4" t="s">
@@ -1882,21 +1916,21 @@
       <c r="A35" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B35" s="12">
+      <c r="B35" s="11">
         <f t="shared" si="2"/>
         <v>-5.1150000000000001E-2</v>
       </c>
-      <c r="C35" s="12">
+      <c r="C35" s="11">
         <v>-0.1023</v>
       </c>
-      <c r="D35" s="12">
+      <c r="D35" s="11">
         <f t="shared" si="3"/>
         <v>-0.15345</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="F35" s="11" t="s">
+      <c r="F35" s="10" t="s">
         <v>88</v>
       </c>
       <c r="G35" s="4" t="s">
@@ -1910,21 +1944,21 @@
       <c r="A36" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B36" s="12">
+      <c r="B36" s="11">
         <f t="shared" si="2"/>
         <v>-2.8500000000000001E-3</v>
       </c>
-      <c r="C36" s="12">
+      <c r="C36" s="11">
         <v>-5.7000000000000002E-3</v>
       </c>
-      <c r="D36" s="12">
+      <c r="D36" s="11">
         <f t="shared" si="3"/>
         <v>-8.5500000000000003E-3</v>
       </c>
       <c r="E36" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="F36" s="11" t="s">
+      <c r="F36" s="10" t="s">
         <v>88</v>
       </c>
       <c r="G36" s="4" t="s">
@@ -1938,21 +1972,21 @@
       <c r="A37" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B37" s="12">
+      <c r="B37" s="11">
         <f t="shared" si="2"/>
         <v>-2.5999999999999998E-4</v>
       </c>
-      <c r="C37" s="12">
+      <c r="C37" s="11">
         <v>-5.1999999999999995E-4</v>
       </c>
-      <c r="D37" s="12">
+      <c r="D37" s="11">
         <f t="shared" si="3"/>
         <v>-7.7999999999999988E-4</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="F37" s="11" t="s">
+      <c r="F37" s="10" t="s">
         <v>88</v>
       </c>
       <c r="G37" s="4" t="s">
@@ -1966,21 +2000,21 @@
       <c r="A38" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B38" s="12">
+      <c r="B38" s="11">
         <f t="shared" si="2"/>
         <v>-2.5999999999999998E-4</v>
       </c>
-      <c r="C38" s="12">
+      <c r="C38" s="11">
         <v>-5.1999999999999995E-4</v>
       </c>
-      <c r="D38" s="12">
+      <c r="D38" s="11">
         <f t="shared" si="3"/>
         <v>-7.7999999999999988E-4</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="F38" s="11" t="s">
+      <c r="F38" s="10" t="s">
         <v>88</v>
       </c>
       <c r="G38" s="4" t="s">
@@ -1994,21 +2028,21 @@
       <c r="A39" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B39" s="12">
+      <c r="B39" s="11">
         <f t="shared" si="2"/>
         <v>-3.0499999999999999E-4</v>
       </c>
-      <c r="C39" s="12">
+      <c r="C39" s="11">
         <v>-6.0999999999999997E-4</v>
       </c>
-      <c r="D39" s="12">
+      <c r="D39" s="11">
         <f t="shared" si="3"/>
         <v>-9.1500000000000001E-4</v>
       </c>
       <c r="E39" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="F39" s="11" t="s">
+      <c r="F39" s="10" t="s">
         <v>88</v>
       </c>
       <c r="G39" s="4" t="s">
@@ -2022,21 +2056,21 @@
       <c r="A40" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B40" s="12">
+      <c r="B40" s="11">
         <f t="shared" si="2"/>
         <v>-3.0499999999999999E-4</v>
       </c>
-      <c r="C40" s="12">
+      <c r="C40" s="11">
         <v>-6.0999999999999997E-4</v>
       </c>
-      <c r="D40" s="12">
+      <c r="D40" s="11">
         <f t="shared" si="3"/>
         <v>-9.1500000000000001E-4</v>
       </c>
       <c r="E40" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="F40" s="11" t="s">
+      <c r="F40" s="10" t="s">
         <v>88</v>
       </c>
       <c r="G40" s="4" t="s">
@@ -2050,21 +2084,21 @@
       <c r="A41" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B41" s="12">
+      <c r="B41" s="11">
         <f t="shared" si="2"/>
         <v>-3.6999999999999999E-4</v>
       </c>
-      <c r="C41" s="12">
+      <c r="C41" s="11">
         <v>-7.3999999999999999E-4</v>
       </c>
-      <c r="D41" s="12">
+      <c r="D41" s="11">
         <f t="shared" si="3"/>
         <v>-1.1099999999999999E-3</v>
       </c>
       <c r="E41" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="F41" s="11" t="s">
+      <c r="F41" s="10" t="s">
         <v>88</v>
       </c>
       <c r="G41" s="4" t="s">
@@ -2082,7 +2116,7 @@
         <f t="shared" si="2"/>
         <v>1.65E-3</v>
       </c>
-      <c r="C42" s="13">
+      <c r="C42" s="12">
         <v>3.3E-3</v>
       </c>
       <c r="D42" s="5">
@@ -2092,13 +2126,13 @@
       <c r="E42" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="F42" s="11" t="s">
+      <c r="F42" s="10" t="s">
         <v>88</v>
       </c>
       <c r="G42" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="H42" s="11" t="s">
+      <c r="H42" s="10" t="s">
         <v>92</v>
       </c>
     </row>
@@ -2110,7 +2144,7 @@
         <f t="shared" si="2"/>
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="C43" s="13">
+      <c r="C43" s="12">
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="D43" s="5">
@@ -2120,13 +2154,13 @@
       <c r="E43" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="F43" s="11" t="s">
+      <c r="F43" s="10" t="s">
         <v>88</v>
       </c>
       <c r="G43" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="H43" s="11" t="s">
+      <c r="H43" s="10" t="s">
         <v>92</v>
       </c>
     </row>
@@ -2134,25 +2168,25 @@
       <c r="A44" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B44" s="13">
+      <c r="B44" s="12">
         <v>0</v>
       </c>
-      <c r="C44" s="13">
+      <c r="C44" s="12">
         <v>0.5</v>
       </c>
-      <c r="D44" s="13">
+      <c r="D44" s="12">
         <v>0.9</v>
       </c>
       <c r="E44" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="F44" s="11" t="s">
+      <c r="F44" s="10" t="s">
         <v>88</v>
       </c>
       <c r="G44" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="H44" s="11" t="s">
+      <c r="H44" s="10" t="s">
         <v>90</v>
       </c>
     </row>
@@ -2178,33 +2212,33 @@
       <c r="G45" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="H45" s="11" t="s">
+      <c r="H45" s="10" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="6" t="s">
+      <c r="A46" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="B46" s="15">
+      <c r="B46" s="16">
         <v>250</v>
       </c>
-      <c r="C46" s="15">
+      <c r="C46" s="16">
         <v>1000</v>
       </c>
-      <c r="D46" s="15">
+      <c r="D46" s="16">
         <v>2500</v>
       </c>
-      <c r="E46" s="7" t="s">
+      <c r="E46" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="F46" s="8" t="s">
+      <c r="F46" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="G46" s="7" t="s">
+      <c r="G46" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="H46" s="11" t="s">
+      <c r="H46" s="10" t="s">
         <v>126</v>
       </c>
     </row>
@@ -2212,13 +2246,13 @@
       <c r="A47" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B47" s="14">
+      <c r="B47" s="13">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="C47" s="14">
+      <c r="C47" s="13">
         <v>0.127</v>
       </c>
-      <c r="D47" s="14">
+      <c r="D47" s="13">
         <v>0.23599999999999999</v>
       </c>
       <c r="E47" s="3" t="s">
@@ -2238,13 +2272,13 @@
       <c r="A48" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B48" s="14">
+      <c r="B48" s="13">
         <v>5.5E-2</v>
       </c>
-      <c r="C48" s="14">
+      <c r="C48" s="13">
         <v>9.8999999999999977E-2</v>
       </c>
-      <c r="D48" s="14">
+      <c r="D48" s="13">
         <v>0.14299999999999999</v>
       </c>
       <c r="E48" s="3" t="s">
@@ -2264,13 +2298,13 @@
       <c r="A49" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B49" s="14">
+      <c r="B49" s="13">
         <v>5.5E-2</v>
       </c>
-      <c r="C49" s="14">
+      <c r="C49" s="13">
         <v>9.8999999999999977E-2</v>
       </c>
-      <c r="D49" s="14">
+      <c r="D49" s="13">
         <v>0.14299999999999999</v>
       </c>
       <c r="E49" s="3" t="s">
@@ -2290,13 +2324,13 @@
       <c r="A50" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B50" s="14">
+      <c r="B50" s="13">
         <v>5.5E-2</v>
       </c>
-      <c r="C50" s="14">
+      <c r="C50" s="13">
         <v>9.8999999999999977E-2</v>
       </c>
-      <c r="D50" s="14">
+      <c r="D50" s="13">
         <v>0.14299999999999999</v>
       </c>
       <c r="E50" s="3" t="s">
@@ -2316,13 +2350,13 @@
       <c r="A51" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B51" s="14">
+      <c r="B51" s="13">
         <v>5.5E-2</v>
       </c>
-      <c r="C51" s="14">
+      <c r="C51" s="13">
         <v>9.8999999999999977E-2</v>
       </c>
-      <c r="D51" s="14">
+      <c r="D51" s="13">
         <v>0.14299999999999999</v>
       </c>
       <c r="E51" s="3" t="s">
@@ -2342,13 +2376,13 @@
       <c r="A52" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="B52" s="14">
+      <c r="B52" s="13">
         <v>8.2000000000000003E-2</v>
       </c>
-      <c r="C52" s="14">
+      <c r="C52" s="13">
         <v>0.27200000000000002</v>
       </c>
-      <c r="D52" s="14">
+      <c r="D52" s="13">
         <v>0.49399999999999999</v>
       </c>
       <c r="E52" s="3" t="s">
@@ -2368,13 +2402,13 @@
       <c r="A53" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B53" s="14">
+      <c r="B53" s="13">
         <v>5.5E-2</v>
       </c>
-      <c r="C53" s="14">
+      <c r="C53" s="13">
         <v>9.8999999999999977E-2</v>
       </c>
-      <c r="D53" s="14">
+      <c r="D53" s="13">
         <v>0.14299999999999999</v>
       </c>
       <c r="E53" s="3" t="s">
@@ -2394,13 +2428,13 @@
       <c r="A54" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B54" s="14">
+      <c r="B54" s="13">
         <v>5.5E-2</v>
       </c>
-      <c r="C54" s="14">
+      <c r="C54" s="13">
         <v>9.8999999999999977E-2</v>
       </c>
-      <c r="D54" s="14">
+      <c r="D54" s="13">
         <v>0.14299999999999999</v>
       </c>
       <c r="E54" s="3" t="s">
@@ -2420,13 +2454,13 @@
       <c r="A55" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B55" s="14">
+      <c r="B55" s="13">
         <v>5.5E-2</v>
       </c>
-      <c r="C55" s="14">
+      <c r="C55" s="13">
         <v>9.8999999999999977E-2</v>
       </c>
-      <c r="D55" s="14">
+      <c r="D55" s="13">
         <v>0.14299999999999999</v>
       </c>
       <c r="E55" s="3" t="s">
@@ -2446,13 +2480,13 @@
       <c r="A56" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="B56" s="14">
+      <c r="B56" s="13">
         <v>-1.0999999999999999E-2</v>
       </c>
-      <c r="C56" s="14">
+      <c r="C56" s="13">
         <v>2.8000000000000025E-2</v>
       </c>
-      <c r="D56" s="14">
+      <c r="D56" s="13">
         <v>7.0999999999999994E-2</v>
       </c>
       <c r="E56" s="3" t="s">
@@ -2472,13 +2506,13 @@
       <c r="A57" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="B57" s="14">
+      <c r="B57" s="13">
         <v>5.5E-2</v>
       </c>
-      <c r="C57" s="14">
+      <c r="C57" s="13">
         <v>9.8999999999999977E-2</v>
       </c>
-      <c r="D57" s="14">
+      <c r="D57" s="13">
         <v>0.14299999999999999</v>
       </c>
       <c r="E57" s="3" t="s">
@@ -2498,13 +2532,13 @@
       <c r="A58" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="B58" s="14">
+      <c r="B58" s="13">
         <v>1.6E-2</v>
       </c>
-      <c r="C58" s="14">
+      <c r="C58" s="13">
         <v>8.0000000000000071E-2</v>
       </c>
-      <c r="D58" s="14">
+      <c r="D58" s="13">
         <v>0.14799999999999999</v>
       </c>
       <c r="E58" s="3" t="s">
@@ -2524,13 +2558,13 @@
       <c r="A59" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="B59" s="14">
+      <c r="B59" s="13">
         <v>4.9000000000000002E-2</v>
       </c>
-      <c r="C59" s="14">
+      <c r="C59" s="13">
         <v>9.8999999999999977E-2</v>
       </c>
-      <c r="D59" s="14">
+      <c r="D59" s="13">
         <v>0.13200000000000001</v>
       </c>
       <c r="E59" s="3" t="s">
@@ -2550,13 +2584,13 @@
       <c r="A60" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="B60" s="14">
+      <c r="B60" s="13">
         <v>5.5E-2</v>
       </c>
-      <c r="C60" s="14">
+      <c r="C60" s="13">
         <v>9.8999999999999977E-2</v>
       </c>
-      <c r="D60" s="14">
+      <c r="D60" s="13">
         <v>0.14299999999999999</v>
       </c>
       <c r="E60" s="3" t="s">
@@ -2576,13 +2610,13 @@
       <c r="A61" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B61" s="14">
+      <c r="B61" s="13">
         <v>5.5E-2</v>
       </c>
-      <c r="C61" s="14">
+      <c r="C61" s="13">
         <v>9.8999999999999977E-2</v>
       </c>
-      <c r="D61" s="14">
+      <c r="D61" s="13">
         <v>0.14299999999999999</v>
       </c>
       <c r="E61" s="3" t="s">
@@ -2602,13 +2636,13 @@
       <c r="A62" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="B62" s="14">
+      <c r="B62" s="13">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="C62" s="14">
+      <c r="C62" s="13">
         <v>0.15900000000000003</v>
       </c>
-      <c r="D62" s="14">
+      <c r="D62" s="13">
         <v>0.36299999999999999</v>
       </c>
       <c r="E62" s="3" t="s">
@@ -2628,15 +2662,15 @@
       <c r="A63" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="B63" s="14">
+      <c r="B63" s="13">
         <f>B56</f>
         <v>-1.0999999999999999E-2</v>
       </c>
-      <c r="C63" s="14">
+      <c r="C63" s="13">
         <f t="shared" ref="C63:D63" si="4">C56</f>
         <v>2.8000000000000025E-2</v>
       </c>
-      <c r="D63" s="14">
+      <c r="D63" s="13">
         <f t="shared" si="4"/>
         <v>7.0999999999999994E-2</v>
       </c>
@@ -2657,13 +2691,13 @@
       <c r="A64" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="B64" s="14">
+      <c r="B64" s="13">
         <v>5.5E-2</v>
       </c>
-      <c r="C64" s="14">
+      <c r="C64" s="13">
         <v>9.8999999999999977E-2</v>
       </c>
-      <c r="D64" s="14">
+      <c r="D64" s="13">
         <v>0.14299999999999999</v>
       </c>
       <c r="E64" s="3" t="s">
@@ -2683,13 +2717,13 @@
       <c r="A65" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="B65" s="14">
+      <c r="B65" s="13">
         <v>5.5E-2</v>
       </c>
-      <c r="C65" s="14">
+      <c r="C65" s="13">
         <v>9.8999999999999977E-2</v>
       </c>
-      <c r="D65" s="14">
+      <c r="D65" s="13">
         <v>0.14299999999999999</v>
       </c>
       <c r="E65" s="3" t="s">
@@ -2709,13 +2743,13 @@
       <c r="A66" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="B66" s="14">
+      <c r="B66" s="13">
         <v>5.5E-2</v>
       </c>
-      <c r="C66" s="14">
+      <c r="C66" s="13">
         <v>9.8999999999999977E-2</v>
       </c>
-      <c r="D66" s="14">
+      <c r="D66" s="13">
         <v>0.14299999999999999</v>
       </c>
       <c r="E66" s="3" t="s">
@@ -2735,4 +2769,84 @@
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAF4C056-73DD-4AC5-8BE4-76E3645E3B7C}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>136</v>
+      </c>
+      <c r="B6" t="s">
+        <v>134</v>
+      </c>
+      <c r="C6" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
error in GCAM - missing AGR emissions for biochar lands
</commit_message>
<xml_diff>
--- a/gcam/input/biochar_land_R/GCAM_parameters.xlsx
+++ b/gcam/input/biochar_land_R/GCAM_parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natha\PycharmProjects\IAM\biochar\gcam\input\biochar_land_R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D01F8A64-D62F-4CA1-AD07-E7B48831D201}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B772223F-3692-46E7-ADE6-6381B4ECEC53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{D3FBB104-BEF4-4FDA-A1FA-9751FB33CA85}"/>
   </bookViews>
@@ -441,9 +441,6 @@
     <t>BiocharYieldHigh</t>
   </si>
   <si>
-    <t>running</t>
-  </si>
-  <si>
     <t>BiocharYieldLow</t>
   </si>
   <si>
@@ -451,6 +448,9 @@
   </si>
   <si>
     <t>NutrientYieldHigh</t>
+  </si>
+  <si>
+    <t>stopped due to error in agr emissions</t>
   </si>
 </sst>
 </file>
@@ -965,7 +965,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FC7B4C1-BB5E-45EB-9034-E2CB0DD15D7E}">
   <dimension ref="A1:H66"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A35" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
@@ -2776,7 +2776,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2821,7 +2821,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B5" t="s">
         <v>132</v>
@@ -2832,18 +2832,18 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B6" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C6" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
biochar high cost 6p0 data
</commit_message>
<xml_diff>
--- a/gcam/input/biochar_land_R/GCAM_parameters.xlsx
+++ b/gcam/input/biochar_land_R/GCAM_parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natha\PycharmProjects\IAM\biochar\gcam\input\biochar_land_R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B772223F-3692-46E7-ADE6-6381B4ECEC53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBFD899B-90CE-4C90-8742-625F5E702F48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{D3FBB104-BEF4-4FDA-A1FA-9751FB33CA85}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="136">
   <si>
     <t>Name</t>
   </si>
@@ -438,19 +438,13 @@
     <t>no</t>
   </si>
   <si>
-    <t>BiocharYieldHigh</t>
-  </si>
-  <si>
-    <t>BiocharYieldLow</t>
-  </si>
-  <si>
-    <t>NutrientYieldLow</t>
-  </si>
-  <si>
-    <t>NutrientYieldHigh</t>
-  </si>
-  <si>
-    <t>stopped due to error in agr emissions</t>
+    <t>HighBiocharCost</t>
+  </si>
+  <si>
+    <t>running</t>
+  </si>
+  <si>
+    <t>LowBiocharCost</t>
   </si>
 </sst>
 </file>
@@ -2773,10 +2767,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAF4C056-73DD-4AC5-8BE4-76E3645E3B7C}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2821,29 +2815,13 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C5" t="s">
         <v>134</v>
-      </c>
-      <c r="B5" t="s">
-        <v>132</v>
-      </c>
-      <c r="C5" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>135</v>
-      </c>
-      <c r="B6" t="s">
-        <v>131</v>
-      </c>
-      <c r="C6" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sensitivity analysis config changes
</commit_message>
<xml_diff>
--- a/gcam/input/biochar_land_R/GCAM_parameters.xlsx
+++ b/gcam/input/biochar_land_R/GCAM_parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natha\PycharmProjects\IAM\biochar\gcam\input\biochar_land_R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D15852F2-2B90-4C36-820F-90A569F47DC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0E61F94-445D-4BAA-A2E5-F3E481436A14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="17385" activeTab="1" xr2:uid="{D3FBB104-BEF4-4FDA-A1FA-9751FB33CA85}"/>
   </bookViews>
@@ -2797,7 +2797,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2863,7 +2863,7 @@
         <v>131</v>
       </c>
       <c r="C6" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -2871,10 +2871,10 @@
         <v>136</v>
       </c>
       <c r="B7" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="C7" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updates to sensitivity analysis
</commit_message>
<xml_diff>
--- a/gcam/input/biochar_land_R/GCAM_parameters.xlsx
+++ b/gcam/input/biochar_land_R/GCAM_parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natha\PycharmProjects\IAM\biochar\gcam\input\biochar_land_R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0E61F94-445D-4BAA-A2E5-F3E481436A14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CFCC427-A3DC-4A9A-976B-3B6210E2E9D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="17385" activeTab="1" xr2:uid="{D3FBB104-BEF4-4FDA-A1FA-9751FB33CA85}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="146">
   <si>
     <t>Name</t>
   </si>
@@ -472,6 +472,9 @@
   </si>
   <si>
     <t>GCAMLandSharesHigh</t>
+  </si>
+  <si>
+    <t>added to db</t>
   </si>
 </sst>
 </file>
@@ -2797,7 +2800,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2827,7 +2830,7 @@
         <v>130</v>
       </c>
       <c r="B3" t="s">
-        <v>131</v>
+        <v>145</v>
       </c>
       <c r="C3" t="s">
         <v>141</v>
@@ -2838,7 +2841,7 @@
         <v>132</v>
       </c>
       <c r="B4" t="s">
-        <v>131</v>
+        <v>145</v>
       </c>
       <c r="C4" t="s">
         <v>141</v>
@@ -2849,7 +2852,7 @@
         <v>134</v>
       </c>
       <c r="B5" t="s">
-        <v>131</v>
+        <v>145</v>
       </c>
       <c r="C5" t="s">
         <v>141</v>
@@ -2860,7 +2863,7 @@
         <v>135</v>
       </c>
       <c r="B6" t="s">
-        <v>131</v>
+        <v>145</v>
       </c>
       <c r="C6" t="s">
         <v>141</v>
@@ -2871,10 +2874,10 @@
         <v>136</v>
       </c>
       <c r="B7" t="s">
-        <v>131</v>
+        <v>145</v>
       </c>
       <c r="C7" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2882,10 +2885,10 @@
         <v>137</v>
       </c>
       <c r="B8" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="C8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -2893,10 +2896,10 @@
         <v>138</v>
       </c>
       <c r="B9" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="C9" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
high cost data output
</commit_message>
<xml_diff>
--- a/gcam/input/biochar_land_R/GCAM_parameters.xlsx
+++ b/gcam/input/biochar_land_R/GCAM_parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natha\PycharmProjects\IAM\biochar\gcam\input\biochar_land_R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CFCC427-A3DC-4A9A-976B-3B6210E2E9D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1F4EFD3-9F76-4490-8E6D-DDBBB07B06DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="17385" activeTab="1" xr2:uid="{D3FBB104-BEF4-4FDA-A1FA-9751FB33CA85}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="148">
   <si>
     <t>Name</t>
   </si>
@@ -475,6 +475,12 @@
   </si>
   <si>
     <t>added to db</t>
+  </si>
+  <si>
+    <t>GCAMManurePriceLow</t>
+  </si>
+  <si>
+    <t>GCAMManurePriceHigh</t>
   </si>
 </sst>
 </file>
@@ -2797,10 +2803,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAF4C056-73DD-4AC5-8BE4-76E3645E3B7C}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2946,6 +2952,16 @@
         <v>142</v>
       </c>
     </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>147</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
new sensitivity config files
</commit_message>
<xml_diff>
--- a/gcam/input/biochar_land_R/GCAM_parameters.xlsx
+++ b/gcam/input/biochar_land_R/GCAM_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natha\PycharmProjects\IAM\biochar\gcam\input\biochar_land_R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{638EF33A-72F7-4391-9ACF-AB647253248E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{354449BA-DFC0-4909-B53D-3D85A80CEAD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="17385" activeTab="1" xr2:uid="{D3FBB104-BEF4-4FDA-A1FA-9751FB33CA85}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{D3FBB104-BEF4-4FDA-A1FA-9751FB33CA85}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="148">
   <si>
     <t>Name</t>
   </si>
@@ -447,12 +447,6 @@
     <t>BiocharNutrientsLow</t>
   </si>
   <si>
-    <t>error</t>
-  </si>
-  <si>
-    <t>not started</t>
-  </si>
-  <si>
     <t>GCAMLandSharesLow</t>
   </si>
   <si>
@@ -468,6 +462,9 @@
     <t>GCAMManurePriceHigh</t>
   </si>
   <si>
+    <t>run</t>
+  </si>
+  <si>
     <t>HighCropYield</t>
   </si>
   <si>
@@ -481,6 +478,9 @@
   </si>
   <si>
     <t>output .csvs</t>
+  </si>
+  <si>
+    <t>A_an_secout_prices</t>
   </si>
 </sst>
 </file>
@@ -605,7 +605,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -656,6 +656,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -993,10 +996,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FC7B4C1-BB5E-45EB-9034-E2CB0DD15D7E}">
-  <dimension ref="A1:H66"/>
+  <dimension ref="A1:H67"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2224,17 +2227,17 @@
       <c r="A45" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B45" s="8">
+      <c r="B45" s="18">
+        <v>1E-3</v>
+      </c>
+      <c r="C45" s="18">
         <v>0.01</v>
       </c>
-      <c r="C45" s="8">
-        <v>0.05</v>
-      </c>
-      <c r="D45" s="8">
+      <c r="D45" s="18">
         <v>0.1</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>41</v>
+        <v>87</v>
       </c>
       <c r="F45" s="8" t="s">
         <v>87</v>
@@ -2243,73 +2246,73 @@
         <v>75</v>
       </c>
       <c r="H45" s="10" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B46" s="8">
+        <v>0.04</v>
+      </c>
+      <c r="C46" s="8">
+        <v>0.05</v>
+      </c>
+      <c r="D46" s="8">
+        <v>0.06</v>
+      </c>
+      <c r="E46" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F46" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="G46" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="H46" s="10" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="14" t="s">
+    <row r="47" spans="1:8" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="B46" s="16">
+      <c r="B47" s="16">
         <v>250</v>
       </c>
-      <c r="C46" s="16">
+      <c r="C47" s="16">
         <v>1000</v>
       </c>
-      <c r="D46" s="16">
+      <c r="D47" s="16">
         <v>2500</v>
       </c>
-      <c r="E46" s="10" t="s">
+      <c r="E47" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="F46" s="17" t="s">
+      <c r="F47" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="G46" s="10" t="s">
+      <c r="G47" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="H46" s="10" t="s">
+      <c r="H47" s="10" t="s">
         <v>126</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="B47" s="13">
-        <v>2.1999999999999999E-2</v>
-      </c>
-      <c r="C47" s="13">
-        <v>0.127</v>
-      </c>
-      <c r="D47" s="13">
-        <v>0.23599999999999999</v>
-      </c>
-      <c r="E47" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="F47" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="G47" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="H47" s="3" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B48" s="13">
-        <v>5.5E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="C48" s="13">
-        <v>9.8999999999999977E-2</v>
+        <v>0.127</v>
       </c>
       <c r="D48" s="13">
-        <v>0.14299999999999999</v>
+        <v>0.23599999999999999</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>41</v>
@@ -2326,7 +2329,7 @@
     </row>
     <row r="49" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B49" s="13">
         <v>5.5E-2</v>
@@ -2352,7 +2355,7 @@
     </row>
     <row r="50" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B50" s="13">
         <v>5.5E-2</v>
@@ -2378,7 +2381,7 @@
     </row>
     <row r="51" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B51" s="13">
         <v>5.5E-2</v>
@@ -2404,16 +2407,16 @@
     </row>
     <row r="52" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B52" s="13">
-        <v>8.2000000000000003E-2</v>
+        <v>5.5E-2</v>
       </c>
       <c r="C52" s="13">
-        <v>0.27200000000000002</v>
+        <v>9.8999999999999977E-2</v>
       </c>
       <c r="D52" s="13">
-        <v>0.49399999999999999</v>
+        <v>0.14299999999999999</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>41</v>
@@ -2430,16 +2433,16 @@
     </row>
     <row r="53" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B53" s="13">
-        <v>5.5E-2</v>
+        <v>8.2000000000000003E-2</v>
       </c>
       <c r="C53" s="13">
-        <v>9.8999999999999977E-2</v>
+        <v>0.27200000000000002</v>
       </c>
       <c r="D53" s="13">
-        <v>0.14299999999999999</v>
+        <v>0.49399999999999999</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>41</v>
@@ -2456,7 +2459,7 @@
     </row>
     <row r="54" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B54" s="13">
         <v>5.5E-2</v>
@@ -2482,7 +2485,7 @@
     </row>
     <row r="55" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B55" s="13">
         <v>5.5E-2</v>
@@ -2508,16 +2511,16 @@
     </row>
     <row r="56" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B56" s="13">
-        <v>-1.0999999999999999E-2</v>
+        <v>5.5E-2</v>
       </c>
       <c r="C56" s="13">
-        <v>2.8000000000000025E-2</v>
+        <v>9.8999999999999977E-2</v>
       </c>
       <c r="D56" s="13">
-        <v>7.0999999999999994E-2</v>
+        <v>0.14299999999999999</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>41</v>
@@ -2534,16 +2537,16 @@
     </row>
     <row r="57" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B57" s="13">
-        <v>5.5E-2</v>
+        <v>-1.0999999999999999E-2</v>
       </c>
       <c r="C57" s="13">
-        <v>9.8999999999999977E-2</v>
+        <v>2.8000000000000025E-2</v>
       </c>
       <c r="D57" s="13">
-        <v>0.14299999999999999</v>
+        <v>7.0999999999999994E-2</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>41</v>
@@ -2560,16 +2563,16 @@
     </row>
     <row r="58" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B58" s="13">
-        <v>1.6E-2</v>
+        <v>5.5E-2</v>
       </c>
       <c r="C58" s="13">
-        <v>8.0000000000000071E-2</v>
+        <v>9.8999999999999977E-2</v>
       </c>
       <c r="D58" s="13">
-        <v>0.14799999999999999</v>
+        <v>0.14299999999999999</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>41</v>
@@ -2586,16 +2589,16 @@
     </row>
     <row r="59" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B59" s="13">
-        <v>4.9000000000000002E-2</v>
+        <v>1.6E-2</v>
       </c>
       <c r="C59" s="13">
-        <v>9.8999999999999977E-2</v>
+        <v>8.0000000000000071E-2</v>
       </c>
       <c r="D59" s="13">
-        <v>0.13200000000000001</v>
+        <v>0.14799999999999999</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>41</v>
@@ -2612,16 +2615,16 @@
     </row>
     <row r="60" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B60" s="13">
-        <v>5.5E-2</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="C60" s="13">
         <v>9.8999999999999977E-2</v>
       </c>
       <c r="D60" s="13">
-        <v>0.14299999999999999</v>
+        <v>0.13200000000000001</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>41</v>
@@ -2638,7 +2641,7 @@
     </row>
     <row r="61" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B61" s="13">
         <v>5.5E-2</v>
@@ -2664,16 +2667,16 @@
     </row>
     <row r="62" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B62" s="13">
-        <v>5.0000000000000001E-3</v>
+        <v>5.5E-2</v>
       </c>
       <c r="C62" s="13">
-        <v>0.15900000000000003</v>
+        <v>9.8999999999999977E-2</v>
       </c>
       <c r="D62" s="13">
-        <v>0.36299999999999999</v>
+        <v>0.14299999999999999</v>
       </c>
       <c r="E62" s="3" t="s">
         <v>41</v>
@@ -2690,46 +2693,46 @@
     </row>
     <row r="63" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B63" s="13">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C63" s="13">
+        <v>0.15900000000000003</v>
+      </c>
+      <c r="D63" s="13">
+        <v>0.36299999999999999</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F63" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="G63" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="H63" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="B63" s="13">
-        <f>B56</f>
+      <c r="B64" s="13">
+        <f>B57</f>
         <v>-1.0999999999999999E-2</v>
       </c>
-      <c r="C63" s="13">
-        <f t="shared" ref="C63:D63" si="4">C56</f>
+      <c r="C64" s="13">
+        <f t="shared" ref="C64:D64" si="4">C57</f>
         <v>2.8000000000000025E-2</v>
       </c>
-      <c r="D63" s="13">
+      <c r="D64" s="13">
         <f t="shared" si="4"/>
         <v>7.0999999999999994E-2</v>
       </c>
-      <c r="E63" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="F63" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="G63" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="H63" s="3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="B64" s="13">
-        <v>5.5E-2</v>
-      </c>
-      <c r="C64" s="13">
-        <v>9.8999999999999977E-2</v>
-      </c>
-      <c r="D64" s="13">
-        <v>0.14299999999999999</v>
-      </c>
       <c r="E64" s="3" t="s">
         <v>41</v>
       </c>
@@ -2745,7 +2748,7 @@
     </row>
     <row r="65" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B65" s="13">
         <v>5.5E-2</v>
@@ -2771,7 +2774,7 @@
     </row>
     <row r="66" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B66" s="13">
         <v>5.5E-2</v>
@@ -2792,6 +2795,32 @@
         <v>83</v>
       </c>
       <c r="H66" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B67" s="13">
+        <v>5.5E-2</v>
+      </c>
+      <c r="C67" s="13">
+        <v>9.8999999999999977E-2</v>
+      </c>
+      <c r="D67" s="13">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F67" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="G67" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="H67" s="3" t="s">
         <v>117</v>
       </c>
     </row>
@@ -2805,8 +2834,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAF4C056-73DD-4AC5-8BE4-76E3645E3B7C}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2830,10 +2859,10 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2841,7 +2870,7 @@
         <v>129</v>
       </c>
       <c r="B4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2849,7 +2878,7 @@
         <v>131</v>
       </c>
       <c r="B5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -2857,7 +2886,7 @@
         <v>132</v>
       </c>
       <c r="B6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -2865,20 +2894,20 @@
         <v>133</v>
       </c>
       <c r="B7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B8" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B9" t="s">
         <v>130</v>
@@ -2889,7 +2918,7 @@
         <v>134</v>
       </c>
       <c r="B10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -2897,47 +2926,47 @@
         <v>135</v>
       </c>
       <c r="B11" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>136</v>
+      </c>
+      <c r="B12" t="s">
         <v>138</v>
-      </c>
-      <c r="B12" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B13" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>139</v>
+      </c>
+      <c r="B14" t="s">
         <v>141</v>
-      </c>
-      <c r="B14" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B15" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>145</v>
+      </c>
+      <c r="B16" t="s">
         <v>146</v>
-      </c>
-      <c r="B16" t="s">
-        <v>147</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes to plots of sensitivity analysis
</commit_message>
<xml_diff>
--- a/gcam/input/biochar_land_R/GCAM_parameters.xlsx
+++ b/gcam/input/biochar_land_R/GCAM_parameters.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natha\PycharmProjects\IAM\biochar\gcam\input\biochar_land_R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{354449BA-DFC0-4909-B53D-3D85A80CEAD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A7E9311-80EF-4334-A7FE-9204CFC418E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{D3FBB104-BEF4-4FDA-A1FA-9751FB33CA85}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="9810" windowHeight="17385" activeTab="1" xr2:uid="{D3FBB104-BEF4-4FDA-A1FA-9751FB33CA85}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="parameter values" sheetId="1" r:id="rId1"/>
+    <sheet name="scenario tracker" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="145">
   <si>
     <t>Name</t>
   </si>
@@ -429,9 +429,6 @@
     <t>HighBiocharCost</t>
   </si>
   <si>
-    <t>running</t>
-  </si>
-  <si>
     <t>LowBiocharCost</t>
   </si>
   <si>
@@ -453,16 +450,10 @@
     <t>GCAMLandSharesHigh</t>
   </si>
   <si>
-    <t>added to db</t>
-  </si>
-  <si>
     <t>GCAMManurePriceLow</t>
   </si>
   <si>
     <t>GCAMManurePriceHigh</t>
-  </si>
-  <si>
-    <t>run</t>
   </si>
   <si>
     <t>HighCropYield</t>
@@ -998,7 +989,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FC7B4C1-BB5E-45EB-9034-E2CB0DD15D7E}">
   <dimension ref="A1:H67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A40" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
@@ -2246,7 +2237,7 @@
         <v>75</v>
       </c>
       <c r="H45" s="10" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -2834,8 +2825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAF4C056-73DD-4AC5-8BE4-76E3645E3B7C}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2859,10 +2850,10 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B3" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2870,103 +2861,103 @@
         <v>129</v>
       </c>
       <c r="B4" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B5" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B6" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B7" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B8" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>140</v>
+      </c>
+      <c r="B9" t="s">
         <v>143</v>
-      </c>
-      <c r="B9" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B10" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B11" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B12" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B13" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B14" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B15" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B16" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update parameters for new sensitivity analyses - waiting soil n2o
</commit_message>
<xml_diff>
--- a/gcam/input/biochar_land_R/GCAM_parameters.xlsx
+++ b/gcam/input/biochar_land_R/GCAM_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natha\PycharmProjects\IAM\biochar\gcam\input\biochar_land_R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A7E9311-80EF-4334-A7FE-9204CFC418E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDADFA54-398D-44E5-A2A3-82E4050BE4AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="0" windowWidth="9810" windowHeight="17385" activeTab="1" xr2:uid="{D3FBB104-BEF4-4FDA-A1FA-9751FB33CA85}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{D3FBB104-BEF4-4FDA-A1FA-9751FB33CA85}"/>
   </bookViews>
   <sheets>
     <sheet name="parameter values" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="159">
   <si>
     <t>Name</t>
   </si>
@@ -306,9 +306,6 @@
     <t>Woolf, D., Amonette, J. E., Street-Perrott, F. A., Lehmann, J. &amp; Joseph, S. Sustainable biochar to mitigate global climate change. Nat Commun 1, 56 (2010).</t>
   </si>
   <si>
-    <t>Arbitrary min/max value</t>
-  </si>
-  <si>
     <t>L2062</t>
   </si>
   <si>
@@ -423,9 +420,6 @@
     <t>Scenario tracker</t>
   </si>
   <si>
-    <t>6p0</t>
-  </si>
-  <si>
     <t>HighBiocharCost</t>
   </si>
   <si>
@@ -472,6 +466,143 @@
   </si>
   <si>
     <t>A_an_secout_prices</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Borchard, N., Schirrmann, M., Cayuela, M.L., Kammann, C., Wrage-Mönnig, N., Estavillo, J.M., Fuertes-Mendizábal, T., Sigua, G., Spokas, K., Ippolito, J.A. and Novak, J., 2019. Biochar, soil and land-use interactions that reduce nitrate leaching and N2O emissions: a meta-analysis. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Science of the Total Environment</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>651</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, pp.2354-2364.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">He, Y., Zhou, X., Jiang, L., Li, M., Du, Z., Zhou, G., Shao, J., Wang, X., Xu, Z., Hosseini Bai, S. and Wallace, H., 2017. Effects of biochar application on soil greenhouse gas fluxes: A meta‐analysis. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Gcb Bioenergy</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>9</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(4), pp.743-755.</t>
+    </r>
+  </si>
+  <si>
+    <t>Min, mean, max for N2O emissions, figure 2, manure and bio-solids</t>
+  </si>
+  <si>
+    <t>Woolf, D., Amonette, J. E., Street-Perrott, F. A., Lehmann, J. &amp; Joseph, S. Sustainable biochar to mitigate global climate change. Nat Commun 1, 56 (2010).
+Güereña, D., Lehmann, J., Hanley, K., Enders, A., Hyland, C. and Riha, S., 2013. Nitrogen dynamics following field application of biochar in a temperate North American maize-based production system. Plant and soil, 365, pp.239-254.</t>
+  </si>
+  <si>
+    <t>No statistical difference in N losses for fertilizer from Guerena (fig 4, 50% secondary N), 50% baseline from Woolf, 58% from Guerena (fig 4, 100% secondary N)</t>
+  </si>
+  <si>
+    <t>Initial price at which the total amount of manure is supplied</t>
+  </si>
+  <si>
+    <t>GCAM Model Parameter - in line with biomass for bioenergy crops in 2035</t>
+  </si>
+  <si>
+    <t>No changes</t>
+  </si>
+  <si>
+    <t>baseline</t>
+  </si>
+  <si>
+    <t>BiocharNUEHigh</t>
+  </si>
+  <si>
+    <t>BiocharNUELow</t>
+  </si>
+  <si>
+    <t>BiocharSoilN2OHigh</t>
+  </si>
+  <si>
+    <t>BiocharSoilN2OLow</t>
+  </si>
+  <si>
+    <t>waiting on soil N2O flux coefficients</t>
+  </si>
+  <si>
+    <t>R files created</t>
+  </si>
+  <si>
+    <t>waiting on soil N2O flux coefficients, need to make R file</t>
   </si>
 </sst>
 </file>
@@ -483,7 +614,7 @@
     <numFmt numFmtId="165" formatCode="0.00000"/>
     <numFmt numFmtId="166" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -510,8 +641,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -527,6 +666,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -631,9 +776,6 @@
     <xf numFmtId="165" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="166" fontId="2" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -650,6 +792,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -989,8 +1134,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FC7B4C1-BB5E-45EB-9034-E2CB0DD15D7E}">
   <dimension ref="A1:H67"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H45" sqref="H45"/>
+    <sheetView topLeftCell="A39" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1053,10 +1198,10 @@
         <v>72</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1081,10 +1226,10 @@
         <v>72</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1109,10 +1254,10 @@
         <v>72</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1137,10 +1282,10 @@
         <v>72</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1165,10 +1310,10 @@
         <v>72</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1220,10 +1365,10 @@
         <v>80</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
@@ -1248,10 +1393,10 @@
         <v>80</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1305,10 +1450,10 @@
         <v>80</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
@@ -1334,10 +1479,10 @@
         <v>80</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
@@ -1388,10 +1533,10 @@
         <v>85</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H14" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1416,10 +1561,10 @@
         <v>85</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
@@ -1471,7 +1616,7 @@
         <v>11</v>
       </c>
       <c r="H17" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
@@ -1497,7 +1642,7 @@
         <v>11</v>
       </c>
       <c r="H18" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1551,7 +1696,7 @@
         <v>83</v>
       </c>
       <c r="H20" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
@@ -1579,7 +1724,7 @@
         <v>83</v>
       </c>
       <c r="H21" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1713,17 +1858,17 @@
       </c>
     </row>
     <row r="27" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="14" t="s">
-        <v>118</v>
-      </c>
-      <c r="B27" s="15">
+      <c r="A27" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="B27" s="14">
         <f>0.5*C27</f>
         <v>-0.125</v>
       </c>
-      <c r="C27" s="15">
+      <c r="C27" s="14">
         <v>-0.25</v>
       </c>
-      <c r="D27" s="15">
+      <c r="D27" s="14">
         <f>1.5*C27</f>
         <v>-0.375</v>
       </c>
@@ -1734,25 +1879,25 @@
         <v>88</v>
       </c>
       <c r="G27" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H27" s="4" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="14" t="s">
-        <v>119</v>
-      </c>
-      <c r="B28" s="15">
-        <f t="shared" ref="B28:B43" si="2">0.5*C28</f>
+      <c r="A28" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="B28" s="14">
+        <f t="shared" ref="B28:B41" si="2">0.5*C28</f>
         <v>-0.125</v>
       </c>
-      <c r="C28" s="15">
+      <c r="C28" s="14">
         <v>-0.25</v>
       </c>
-      <c r="D28" s="15">
-        <f t="shared" ref="D28:D43" si="3">1.5*C28</f>
+      <c r="D28" s="14">
+        <f t="shared" ref="D28:D41" si="3">1.5*C28</f>
         <v>-0.375</v>
       </c>
       <c r="E28" s="10" t="s">
@@ -1762,24 +1907,24 @@
         <v>88</v>
       </c>
       <c r="G28" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H28" s="4" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="14" t="s">
-        <v>120</v>
-      </c>
-      <c r="B29" s="15">
+      <c r="A29" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="B29" s="14">
         <f t="shared" si="2"/>
         <v>-0.155</v>
       </c>
-      <c r="C29" s="15">
+      <c r="C29" s="14">
         <v>-0.31</v>
       </c>
-      <c r="D29" s="15">
+      <c r="D29" s="14">
         <f t="shared" si="3"/>
         <v>-0.46499999999999997</v>
       </c>
@@ -1790,24 +1935,24 @@
         <v>88</v>
       </c>
       <c r="G29" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H29" s="4" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="B30" s="15">
+      <c r="A30" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="B30" s="14">
         <f t="shared" si="2"/>
         <v>-0.155</v>
       </c>
-      <c r="C30" s="15">
+      <c r="C30" s="14">
         <v>-0.31</v>
       </c>
-      <c r="D30" s="15">
+      <c r="D30" s="14">
         <f t="shared" si="3"/>
         <v>-0.46499999999999997</v>
       </c>
@@ -1818,24 +1963,24 @@
         <v>88</v>
       </c>
       <c r="G30" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H30" s="4" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="14" t="s">
-        <v>122</v>
-      </c>
-      <c r="B31" s="15">
+      <c r="A31" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="B31" s="14">
         <f t="shared" si="2"/>
         <v>-0.14000000000000001</v>
       </c>
-      <c r="C31" s="15">
+      <c r="C31" s="14">
         <v>-0.28000000000000003</v>
       </c>
-      <c r="D31" s="15">
+      <c r="D31" s="14">
         <f t="shared" si="3"/>
         <v>-0.42000000000000004</v>
       </c>
@@ -1846,7 +1991,7 @@
         <v>88</v>
       </c>
       <c r="G31" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H31" s="4" t="s">
         <v>74</v>
@@ -1874,7 +2019,7 @@
         <v>88</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H32" s="4" t="s">
         <v>74</v>
@@ -1902,7 +2047,7 @@
         <v>88</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H33" s="4" t="s">
         <v>74</v>
@@ -1930,7 +2075,7 @@
         <v>88</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H34" s="4" t="s">
         <v>74</v>
@@ -1958,7 +2103,7 @@
         <v>88</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H35" s="4" t="s">
         <v>74</v>
@@ -1986,7 +2131,7 @@
         <v>88</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H36" s="4" t="s">
         <v>74</v>
@@ -2014,7 +2159,7 @@
         <v>88</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H37" s="4" t="s">
         <v>74</v>
@@ -2042,7 +2187,7 @@
         <v>88</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H38" s="4" t="s">
         <v>74</v>
@@ -2070,7 +2215,7 @@
         <v>88</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H39" s="4" t="s">
         <v>74</v>
@@ -2098,7 +2243,7 @@
         <v>88</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H40" s="4" t="s">
         <v>74</v>
@@ -2126,7 +2271,7 @@
         <v>88</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H41" s="4" t="s">
         <v>74</v>
@@ -2137,94 +2282,90 @@
         <v>31</v>
       </c>
       <c r="B42" s="5">
-        <f t="shared" si="2"/>
-        <v>1.65E-3</v>
-      </c>
-      <c r="C42" s="12">
-        <v>3.3E-3</v>
+        <v>0</v>
+      </c>
+      <c r="C42" s="5">
+        <v>0</v>
       </c>
       <c r="D42" s="5">
-        <f t="shared" si="3"/>
-        <v>4.9499999999999995E-3</v>
+        <v>0</v>
       </c>
       <c r="E42" s="4" t="s">
         <v>41</v>
       </c>
       <c r="F42" s="10" t="s">
-        <v>88</v>
+        <v>144</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>116</v>
+        <v>150</v>
       </c>
       <c r="H42" s="10" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="78.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B43" s="5">
-        <f t="shared" si="2"/>
-        <v>1.2500000000000001E-2</v>
-      </c>
-      <c r="C43" s="12">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="D43" s="5">
-        <f t="shared" si="3"/>
-        <v>3.7500000000000006E-2</v>
-      </c>
-      <c r="E43" s="4" t="s">
+      <c r="B43" s="18">
+        <v>-0.13</v>
+      </c>
+      <c r="C43" s="18">
+        <v>-0.3</v>
+      </c>
+      <c r="D43" s="18">
+        <v>-0.44</v>
+      </c>
+      <c r="E43" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="F43" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="G43" s="4" t="s">
-        <v>116</v>
+      <c r="F43" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="G43" s="6" t="s">
+        <v>145</v>
       </c>
       <c r="H43" s="10" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="95.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B44" s="12">
+      <c r="B44" s="8">
         <v>0</v>
       </c>
-      <c r="C44" s="12">
+      <c r="C44" s="8">
         <v>0.5</v>
       </c>
-      <c r="D44" s="12">
-        <v>0.9</v>
-      </c>
-      <c r="E44" s="4" t="s">
+      <c r="D44" s="8">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="E44" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="F44" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="G44" s="4" t="s">
+      <c r="F44" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="G44" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="H44" s="10" t="s">
         <v>89</v>
-      </c>
-      <c r="H44" s="10" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B45" s="18">
+        <v>148</v>
+      </c>
+      <c r="B45" s="17">
         <v>1E-3</v>
       </c>
-      <c r="C45" s="18">
+      <c r="C45" s="17">
         <v>0.01</v>
       </c>
-      <c r="D45" s="18">
+      <c r="D45" s="17">
         <v>0.1</v>
       </c>
       <c r="E45" s="7" t="s">
@@ -2237,7 +2378,7 @@
         <v>75</v>
       </c>
       <c r="H45" s="10" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -2245,7 +2386,7 @@
         <v>34</v>
       </c>
       <c r="B46" s="8">
-        <v>0.04</v>
+        <v>0.01</v>
       </c>
       <c r="C46" s="8">
         <v>0.05</v>
@@ -2260,467 +2401,467 @@
         <v>87</v>
       </c>
       <c r="G46" s="7" t="s">
-        <v>75</v>
+        <v>149</v>
       </c>
       <c r="H46" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="14" t="s">
+      <c r="A47" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B47" s="15">
+        <v>250</v>
+      </c>
+      <c r="C47" s="15">
+        <v>1000</v>
+      </c>
+      <c r="D47" s="15">
+        <v>2500</v>
+      </c>
+      <c r="E47" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="F47" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="G47" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="H47" s="10" t="s">
         <v>125</v>
-      </c>
-      <c r="B47" s="16">
-        <v>250</v>
-      </c>
-      <c r="C47" s="16">
-        <v>1000</v>
-      </c>
-      <c r="D47" s="16">
-        <v>2500</v>
-      </c>
-      <c r="E47" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="F47" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="G47" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="H47" s="10" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="B48" s="13">
+        <v>95</v>
+      </c>
+      <c r="B48" s="12">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="C48" s="13">
+      <c r="C48" s="12">
         <v>0.127</v>
       </c>
-      <c r="D48" s="13">
+      <c r="D48" s="12">
         <v>0.23599999999999999</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>41</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G48" s="4" t="s">
         <v>83</v>
       </c>
       <c r="H48" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="B49" s="13">
+        <v>96</v>
+      </c>
+      <c r="B49" s="12">
         <v>5.5E-2</v>
       </c>
-      <c r="C49" s="13">
+      <c r="C49" s="12">
         <v>9.8999999999999977E-2</v>
       </c>
-      <c r="D49" s="13">
+      <c r="D49" s="12">
         <v>0.14299999999999999</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>41</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G49" s="4" t="s">
         <v>83</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="B50" s="13">
+        <v>97</v>
+      </c>
+      <c r="B50" s="12">
         <v>5.5E-2</v>
       </c>
-      <c r="C50" s="13">
+      <c r="C50" s="12">
         <v>9.8999999999999977E-2</v>
       </c>
-      <c r="D50" s="13">
+      <c r="D50" s="12">
         <v>0.14299999999999999</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>41</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G50" s="4" t="s">
         <v>83</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B51" s="13">
+        <v>98</v>
+      </c>
+      <c r="B51" s="12">
         <v>5.5E-2</v>
       </c>
-      <c r="C51" s="13">
+      <c r="C51" s="12">
         <v>9.8999999999999977E-2</v>
       </c>
-      <c r="D51" s="13">
+      <c r="D51" s="12">
         <v>0.14299999999999999</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>41</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G51" s="4" t="s">
         <v>83</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="B52" s="13">
+        <v>99</v>
+      </c>
+      <c r="B52" s="12">
         <v>5.5E-2</v>
       </c>
-      <c r="C52" s="13">
+      <c r="C52" s="12">
         <v>9.8999999999999977E-2</v>
       </c>
-      <c r="D52" s="13">
+      <c r="D52" s="12">
         <v>0.14299999999999999</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>41</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G52" s="4" t="s">
         <v>83</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B53" s="13">
+        <v>100</v>
+      </c>
+      <c r="B53" s="12">
         <v>8.2000000000000003E-2</v>
       </c>
-      <c r="C53" s="13">
+      <c r="C53" s="12">
         <v>0.27200000000000002</v>
       </c>
-      <c r="D53" s="13">
+      <c r="D53" s="12">
         <v>0.49399999999999999</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>41</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G53" s="4" t="s">
         <v>83</v>
       </c>
       <c r="H53" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="B54" s="13">
+        <v>101</v>
+      </c>
+      <c r="B54" s="12">
         <v>5.5E-2</v>
       </c>
-      <c r="C54" s="13">
+      <c r="C54" s="12">
         <v>9.8999999999999977E-2</v>
       </c>
-      <c r="D54" s="13">
+      <c r="D54" s="12">
         <v>0.14299999999999999</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>41</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G54" s="4" t="s">
         <v>83</v>
       </c>
       <c r="H54" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="B55" s="13">
+        <v>102</v>
+      </c>
+      <c r="B55" s="12">
         <v>5.5E-2</v>
       </c>
-      <c r="C55" s="13">
+      <c r="C55" s="12">
         <v>9.8999999999999977E-2</v>
       </c>
-      <c r="D55" s="13">
+      <c r="D55" s="12">
         <v>0.14299999999999999</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>41</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G55" s="4" t="s">
         <v>83</v>
       </c>
       <c r="H55" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="56" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="B56" s="13">
+        <v>103</v>
+      </c>
+      <c r="B56" s="12">
         <v>5.5E-2</v>
       </c>
-      <c r="C56" s="13">
+      <c r="C56" s="12">
         <v>9.8999999999999977E-2</v>
       </c>
-      <c r="D56" s="13">
+      <c r="D56" s="12">
         <v>0.14299999999999999</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>41</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G56" s="4" t="s">
         <v>83</v>
       </c>
       <c r="H56" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="57" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="B57" s="13">
+        <v>104</v>
+      </c>
+      <c r="B57" s="12">
         <v>-1.0999999999999999E-2</v>
       </c>
-      <c r="C57" s="13">
+      <c r="C57" s="12">
         <v>2.8000000000000025E-2</v>
       </c>
-      <c r="D57" s="13">
+      <c r="D57" s="12">
         <v>7.0999999999999994E-2</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>41</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G57" s="4" t="s">
         <v>83</v>
       </c>
       <c r="H57" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="58" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="B58" s="13">
+        <v>105</v>
+      </c>
+      <c r="B58" s="12">
         <v>5.5E-2</v>
       </c>
-      <c r="C58" s="13">
+      <c r="C58" s="12">
         <v>9.8999999999999977E-2</v>
       </c>
-      <c r="D58" s="13">
+      <c r="D58" s="12">
         <v>0.14299999999999999</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>41</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G58" s="4" t="s">
         <v>83</v>
       </c>
       <c r="H58" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="59" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="B59" s="13">
+        <v>106</v>
+      </c>
+      <c r="B59" s="12">
         <v>1.6E-2</v>
       </c>
-      <c r="C59" s="13">
+      <c r="C59" s="12">
         <v>8.0000000000000071E-2</v>
       </c>
-      <c r="D59" s="13">
+      <c r="D59" s="12">
         <v>0.14799999999999999</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>41</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G59" s="4" t="s">
         <v>83</v>
       </c>
       <c r="H59" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="60" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="B60" s="13">
+        <v>107</v>
+      </c>
+      <c r="B60" s="12">
         <v>4.9000000000000002E-2</v>
       </c>
-      <c r="C60" s="13">
+      <c r="C60" s="12">
         <v>9.8999999999999977E-2</v>
       </c>
-      <c r="D60" s="13">
+      <c r="D60" s="12">
         <v>0.13200000000000001</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>41</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G60" s="4" t="s">
         <v>83</v>
       </c>
       <c r="H60" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="61" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="B61" s="13">
+        <v>108</v>
+      </c>
+      <c r="B61" s="12">
         <v>5.5E-2</v>
       </c>
-      <c r="C61" s="13">
+      <c r="C61" s="12">
         <v>9.8999999999999977E-2</v>
       </c>
-      <c r="D61" s="13">
+      <c r="D61" s="12">
         <v>0.14299999999999999</v>
       </c>
       <c r="E61" s="3" t="s">
         <v>41</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G61" s="4" t="s">
         <v>83</v>
       </c>
       <c r="H61" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="62" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="B62" s="13">
+        <v>109</v>
+      </c>
+      <c r="B62" s="12">
         <v>5.5E-2</v>
       </c>
-      <c r="C62" s="13">
+      <c r="C62" s="12">
         <v>9.8999999999999977E-2</v>
       </c>
-      <c r="D62" s="13">
+      <c r="D62" s="12">
         <v>0.14299999999999999</v>
       </c>
       <c r="E62" s="3" t="s">
         <v>41</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G62" s="4" t="s">
         <v>83</v>
       </c>
       <c r="H62" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="63" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="B63" s="13">
+        <v>110</v>
+      </c>
+      <c r="B63" s="12">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="C63" s="13">
+      <c r="C63" s="12">
         <v>0.15900000000000003</v>
       </c>
-      <c r="D63" s="13">
+      <c r="D63" s="12">
         <v>0.36299999999999999</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>41</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G63" s="4" t="s">
         <v>83</v>
       </c>
       <c r="H63" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="64" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="B64" s="13">
+        <v>111</v>
+      </c>
+      <c r="B64" s="12">
         <f>B57</f>
         <v>-1.0999999999999999E-2</v>
       </c>
-      <c r="C64" s="13">
+      <c r="C64" s="12">
         <f t="shared" ref="C64:D64" si="4">C57</f>
         <v>2.8000000000000025E-2</v>
       </c>
-      <c r="D64" s="13">
+      <c r="D64" s="12">
         <f t="shared" si="4"/>
         <v>7.0999999999999994E-2</v>
       </c>
@@ -2728,91 +2869,91 @@
         <v>41</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G64" s="4" t="s">
         <v>83</v>
       </c>
       <c r="H64" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="65" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="B65" s="13">
+        <v>112</v>
+      </c>
+      <c r="B65" s="12">
         <v>5.5E-2</v>
       </c>
-      <c r="C65" s="13">
+      <c r="C65" s="12">
         <v>9.8999999999999977E-2</v>
       </c>
-      <c r="D65" s="13">
+      <c r="D65" s="12">
         <v>0.14299999999999999</v>
       </c>
       <c r="E65" s="3" t="s">
         <v>41</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G65" s="4" t="s">
         <v>83</v>
       </c>
       <c r="H65" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="66" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="B66" s="13">
+        <v>113</v>
+      </c>
+      <c r="B66" s="12">
         <v>5.5E-2</v>
       </c>
-      <c r="C66" s="13">
+      <c r="C66" s="12">
         <v>9.8999999999999977E-2</v>
       </c>
-      <c r="D66" s="13">
+      <c r="D66" s="12">
         <v>0.14299999999999999</v>
       </c>
       <c r="E66" s="3" t="s">
         <v>41</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G66" s="4" t="s">
         <v>83</v>
       </c>
       <c r="H66" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="67" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="B67" s="13">
+        <v>114</v>
+      </c>
+      <c r="B67" s="12">
         <v>5.5E-2</v>
       </c>
-      <c r="C67" s="13">
+      <c r="C67" s="12">
         <v>9.8999999999999977E-2</v>
       </c>
-      <c r="D67" s="13">
+      <c r="D67" s="12">
         <v>0.14299999999999999</v>
       </c>
       <c r="E67" s="3" t="s">
         <v>41</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G67" s="4" t="s">
         <v>83</v>
       </c>
       <c r="H67" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -2823,10 +2964,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAF4C056-73DD-4AC5-8BE4-76E3645E3B7C}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2837,7 +2978,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -2845,119 +2986,151 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>128</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B3" t="s">
-        <v>143</v>
+        <v>156</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B4" t="s">
-        <v>143</v>
+        <v>157</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B5" t="s">
-        <v>143</v>
+        <v>157</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B6" t="s">
-        <v>143</v>
+        <v>157</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B7" t="s">
-        <v>143</v>
+        <v>157</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B8" t="s">
-        <v>143</v>
+        <v>157</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B9" t="s">
-        <v>143</v>
+        <v>157</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B10" t="s">
-        <v>143</v>
+        <v>157</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B11" t="s">
-        <v>143</v>
+        <v>157</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B12" t="s">
-        <v>143</v>
+        <v>157</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B13" t="s">
-        <v>143</v>
+        <v>157</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B14" t="s">
-        <v>143</v>
+        <v>157</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B15" t="s">
-        <v>143</v>
+        <v>157</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>142</v>
+        <v>152</v>
       </c>
       <c r="B16" t="s">
-        <v>143</v>
+        <v>157</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>153</v>
+      </c>
+      <c r="B17" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>154</v>
+      </c>
+      <c r="B18" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>155</v>
+      </c>
+      <c r="B19" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>140</v>
+      </c>
+      <c r="B20" t="s">
+        <v>141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cleaned up files for running sensitivity analysis
</commit_message>
<xml_diff>
--- a/gcam/input/biochar_land_R/GCAM_parameters.xlsx
+++ b/gcam/input/biochar_land_R/GCAM_parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natha\PycharmProjects\IAM\biochar\gcam\input\biochar_land_R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDADFA54-398D-44E5-A2A3-82E4050BE4AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF8890A5-8404-4BEB-8DE3-1FB1F48C7E9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{D3FBB104-BEF4-4FDA-A1FA-9751FB33CA85}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="157">
   <si>
     <t>Name</t>
   </si>
@@ -466,53 +466,6 @@
   </si>
   <si>
     <t>A_an_secout_prices</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Borchard, N., Schirrmann, M., Cayuela, M.L., Kammann, C., Wrage-Mönnig, N., Estavillo, J.M., Fuertes-Mendizábal, T., Sigua, G., Spokas, K., Ippolito, J.A. and Novak, J., 2019. Biochar, soil and land-use interactions that reduce nitrate leaching and N2O emissions: a meta-analysis. </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Science of the Total Environment</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>651</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, pp.2354-2364.</t>
-    </r>
   </si>
   <si>
     <r>
@@ -596,13 +549,10 @@
     <t>BiocharSoilN2OLow</t>
   </si>
   <si>
-    <t>waiting on soil N2O flux coefficients</t>
-  </si>
-  <si>
     <t>R files created</t>
   </si>
   <si>
-    <t>waiting on soil N2O flux coefficients, need to make R file</t>
+    <t>Cayuela, M.L., Van Zwieten, L., Singh, B.P., Jeffery, S., Roig, A. and Sánchez-Monedero, M.A., 2014. Biochar's role in mitigating soil nitrous oxide emissions: A review and meta-analysis. Agriculture, Ecosystems &amp; Environment, 191, pp.5-16.</t>
   </si>
 </sst>
 </file>
@@ -650,7 +600,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -666,12 +616,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -741,7 +685,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -792,9 +736,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1135,7 +1076,7 @@
   <dimension ref="A1:H67"/>
   <sheetViews>
     <sheetView topLeftCell="A39" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G43" sqref="G43"/>
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2294,36 +2235,36 @@
         <v>41</v>
       </c>
       <c r="F42" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H42" s="10" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="78.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B43" s="18">
-        <v>-0.13</v>
-      </c>
-      <c r="C43" s="18">
-        <v>-0.3</v>
-      </c>
-      <c r="D43" s="18">
-        <v>-0.44</v>
+      <c r="B43" s="8">
+        <v>0.39</v>
+      </c>
+      <c r="C43" s="8">
+        <v>-0.02</v>
+      </c>
+      <c r="D43" s="8">
+        <v>-0.46</v>
       </c>
       <c r="E43" s="6" t="s">
         <v>41</v>
       </c>
       <c r="F43" s="6" t="s">
-        <v>143</v>
+        <v>156</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H43" s="10" t="s">
         <v>91</v>
@@ -2346,10 +2287,10 @@
         <v>41</v>
       </c>
       <c r="F44" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="G44" s="6" t="s">
         <v>146</v>
-      </c>
-      <c r="G44" s="6" t="s">
-        <v>147</v>
       </c>
       <c r="H44" s="10" t="s">
         <v>89</v>
@@ -2357,7 +2298,7 @@
     </row>
     <row r="45" spans="1:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B45" s="17">
         <v>1E-3</v>
@@ -2401,7 +2342,7 @@
         <v>87</v>
       </c>
       <c r="G46" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H46" s="10" t="s">
         <v>92</v>
@@ -2967,7 +2908,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2986,7 +2927,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2994,7 +2935,7 @@
         <v>139</v>
       </c>
       <c r="B3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -3002,7 +2943,7 @@
         <v>127</v>
       </c>
       <c r="B4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -3010,7 +2951,7 @@
         <v>128</v>
       </c>
       <c r="B5" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -3018,7 +2959,7 @@
         <v>129</v>
       </c>
       <c r="B6" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -3026,7 +2967,7 @@
         <v>130</v>
       </c>
       <c r="B7" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -3034,7 +2975,7 @@
         <v>137</v>
       </c>
       <c r="B8" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -3042,7 +2983,7 @@
         <v>138</v>
       </c>
       <c r="B9" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -3050,7 +2991,7 @@
         <v>131</v>
       </c>
       <c r="B10" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -3058,7 +2999,7 @@
         <v>132</v>
       </c>
       <c r="B11" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -3066,7 +3007,7 @@
         <v>133</v>
       </c>
       <c r="B12" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -3074,7 +3015,7 @@
         <v>134</v>
       </c>
       <c r="B13" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -3082,7 +3023,7 @@
         <v>135</v>
       </c>
       <c r="B14" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -3090,39 +3031,39 @@
         <v>136</v>
       </c>
       <c r="B15" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B16" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B17" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B18" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>154</v>
+      </c>
+      <c r="B19" t="s">
         <v>155</v>
-      </c>
-      <c r="B19" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
output from gcam db
</commit_message>
<xml_diff>
--- a/gcam/input/biochar_land_R/GCAM_parameters.xlsx
+++ b/gcam/input/biochar_land_R/GCAM_parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natha\PycharmProjects\IAM\biochar\gcam\input\biochar_land_R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F29C7B2-E97F-45B8-8A96-DDA3B6F1D7ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82547EF6-2B5E-4260-86E0-E43E58F0062D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14655" yWindow="0" windowWidth="14190" windowHeight="17385" activeTab="1" xr2:uid="{D3FBB104-BEF4-4FDA-A1FA-9751FB33CA85}"/>
   </bookViews>
@@ -552,10 +552,10 @@
     <t>error</t>
   </si>
   <si>
-    <t>.xml</t>
-  </si>
-  <si>
     <t>done</t>
+  </si>
+  <si>
+    <t>own db</t>
   </si>
 </sst>
 </file>
@@ -2911,7 +2911,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2938,7 +2938,7 @@
         <v>139</v>
       </c>
       <c r="B3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2946,7 +2946,7 @@
         <v>128</v>
       </c>
       <c r="B4" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2954,7 +2954,7 @@
         <v>127</v>
       </c>
       <c r="B5" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -2962,7 +2962,7 @@
         <v>129</v>
       </c>
       <c r="B6" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -2970,7 +2970,7 @@
         <v>130</v>
       </c>
       <c r="B7" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -2978,7 +2978,7 @@
         <v>137</v>
       </c>
       <c r="B8" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -2986,7 +2986,7 @@
         <v>138</v>
       </c>
       <c r="B9" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -3002,7 +3002,7 @@
         <v>132</v>
       </c>
       <c r="B11" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -3010,7 +3010,7 @@
         <v>133</v>
       </c>
       <c r="B12" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -3018,7 +3018,7 @@
         <v>134</v>
       </c>
       <c r="B13" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -3026,7 +3026,7 @@
         <v>135</v>
       </c>
       <c r="B14" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -3034,7 +3034,7 @@
         <v>136</v>
       </c>
       <c r="B15" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -3042,7 +3042,7 @@
         <v>150</v>
       </c>
       <c r="B16" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -3050,7 +3050,7 @@
         <v>151</v>
       </c>
       <c r="B17" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -3058,7 +3058,7 @@
         <v>152</v>
       </c>
       <c r="B18" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -3066,7 +3066,7 @@
         <v>153</v>
       </c>
       <c r="B19" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -3074,7 +3074,7 @@
         <v>140</v>
       </c>
       <c r="B20" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>